<commit_message>
Error in Increment month application is rectified
</commit_message>
<xml_diff>
--- a/arrear_report.xlsx
+++ b/arrear_report.xlsx
@@ -821,22 +821,22 @@
         <v>6600</v>
       </c>
       <c r="C14" t="n">
-        <v>76000</v>
+        <v>78300</v>
       </c>
       <c r="D14" t="n">
-        <v>78800</v>
+        <v>81200</v>
       </c>
       <c r="E14" t="n">
         <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>85880</v>
+        <v>88479</v>
       </c>
       <c r="G14" t="n">
-        <v>89044</v>
+        <v>91756</v>
       </c>
       <c r="H14" t="n">
-        <v>3164</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="15">
@@ -1157,22 +1157,22 @@
         <v>6600</v>
       </c>
       <c r="C26" t="n">
-        <v>78300</v>
+        <v>80700</v>
       </c>
       <c r="D26" t="n">
-        <v>81200</v>
+        <v>83700</v>
       </c>
       <c r="E26" t="n">
         <v>13</v>
       </c>
       <c r="F26" t="n">
-        <v>88479</v>
+        <v>91191</v>
       </c>
       <c r="G26" t="n">
-        <v>91756</v>
+        <v>94581</v>
       </c>
       <c r="H26" t="n">
-        <v>3277</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="27">
@@ -1493,22 +1493,22 @@
         <v>6600</v>
       </c>
       <c r="C38" t="n">
-        <v>80700</v>
+        <v>83200</v>
       </c>
       <c r="D38" t="n">
-        <v>83700</v>
+        <v>86300</v>
       </c>
       <c r="E38" t="n">
         <v>13</v>
       </c>
       <c r="F38" t="n">
-        <v>91191</v>
+        <v>94016</v>
       </c>
       <c r="G38" t="n">
-        <v>94581</v>
+        <v>97519</v>
       </c>
       <c r="H38" t="n">
-        <v>3390</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="39">
@@ -1829,22 +1829,22 @@
         <v>6600</v>
       </c>
       <c r="C50" t="n">
-        <v>83200</v>
+        <v>85700</v>
       </c>
       <c r="D50" t="n">
-        <v>86300</v>
+        <v>88900</v>
       </c>
       <c r="E50" t="n">
         <v>20</v>
       </c>
       <c r="F50" t="n">
-        <v>99840</v>
+        <v>102840</v>
       </c>
       <c r="G50" t="n">
-        <v>103560</v>
+        <v>106680</v>
       </c>
       <c r="H50" t="n">
-        <v>3720</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="51">
@@ -2165,22 +2165,22 @@
         <v>6600</v>
       </c>
       <c r="C62" t="n">
-        <v>85700</v>
+        <v>88300</v>
       </c>
       <c r="D62" t="n">
-        <v>88900</v>
+        <v>91600</v>
       </c>
       <c r="E62" t="n">
         <v>24</v>
       </c>
       <c r="F62" t="n">
-        <v>106268</v>
+        <v>109492</v>
       </c>
       <c r="G62" t="n">
-        <v>110236</v>
+        <v>113584</v>
       </c>
       <c r="H62" t="n">
-        <v>3968</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="63">
@@ -2498,25 +2498,25 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C74" t="n">
-        <v>96800</v>
+        <v>91000</v>
       </c>
       <c r="D74" t="n">
-        <v>102600</v>
+        <v>94400</v>
       </c>
       <c r="E74" t="n">
         <v>28</v>
       </c>
       <c r="F74" t="n">
-        <v>123904</v>
+        <v>116480</v>
       </c>
       <c r="G74" t="n">
-        <v>131328</v>
+        <v>120832</v>
       </c>
       <c r="H74" t="n">
-        <v>7424</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="75">
@@ -2529,22 +2529,22 @@
         <v>7600</v>
       </c>
       <c r="C75" t="n">
-        <v>99800</v>
+        <v>96800</v>
       </c>
       <c r="D75" t="n">
-        <v>105700</v>
+        <v>102600</v>
       </c>
       <c r="E75" t="n">
         <v>28</v>
       </c>
       <c r="F75" t="n">
-        <v>127744</v>
+        <v>123904</v>
       </c>
       <c r="G75" t="n">
-        <v>135296</v>
+        <v>131328</v>
       </c>
       <c r="H75" t="n">
-        <v>7552</v>
+        <v>7424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Error in Increment month application is rectified-2
</commit_message>
<xml_diff>
--- a/arrear_report.xlsx
+++ b/arrear_report.xlsx
@@ -485,22 +485,22 @@
         <v>6600</v>
       </c>
       <c r="C2" t="n">
-        <v>76000</v>
+        <v>83200</v>
       </c>
       <c r="D2" t="n">
-        <v>78800</v>
+        <v>86300</v>
       </c>
       <c r="E2" t="n">
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>83600</v>
+        <v>91520</v>
       </c>
       <c r="G2" t="n">
-        <v>86680</v>
+        <v>94930</v>
       </c>
       <c r="H2" t="n">
-        <v>3080</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="3">
@@ -513,22 +513,22 @@
         <v>6600</v>
       </c>
       <c r="C3" t="n">
-        <v>76000</v>
+        <v>83200</v>
       </c>
       <c r="D3" t="n">
-        <v>78800</v>
+        <v>86300</v>
       </c>
       <c r="E3" t="n">
         <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>83600</v>
+        <v>91520</v>
       </c>
       <c r="G3" t="n">
-        <v>86680</v>
+        <v>94930</v>
       </c>
       <c r="H3" t="n">
-        <v>3080</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="4">
@@ -541,22 +541,22 @@
         <v>6600</v>
       </c>
       <c r="C4" t="n">
-        <v>76000</v>
+        <v>83200</v>
       </c>
       <c r="D4" t="n">
-        <v>78800</v>
+        <v>86300</v>
       </c>
       <c r="E4" t="n">
         <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>83600</v>
+        <v>91520</v>
       </c>
       <c r="G4" t="n">
-        <v>86680</v>
+        <v>94930</v>
       </c>
       <c r="H4" t="n">
-        <v>3080</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="5">
@@ -569,22 +569,22 @@
         <v>6600</v>
       </c>
       <c r="C5" t="n">
-        <v>76000</v>
+        <v>83200</v>
       </c>
       <c r="D5" t="n">
-        <v>78800</v>
+        <v>86300</v>
       </c>
       <c r="E5" t="n">
         <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>83600</v>
+        <v>91520</v>
       </c>
       <c r="G5" t="n">
-        <v>86680</v>
+        <v>94930</v>
       </c>
       <c r="H5" t="n">
-        <v>3080</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="6">
@@ -597,22 +597,22 @@
         <v>6600</v>
       </c>
       <c r="C6" t="n">
-        <v>76000</v>
+        <v>83200</v>
       </c>
       <c r="D6" t="n">
-        <v>78800</v>
+        <v>86300</v>
       </c>
       <c r="E6" t="n">
         <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>83600</v>
+        <v>91520</v>
       </c>
       <c r="G6" t="n">
-        <v>86680</v>
+        <v>94930</v>
       </c>
       <c r="H6" t="n">
-        <v>3080</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="7">
@@ -625,22 +625,22 @@
         <v>6600</v>
       </c>
       <c r="C7" t="n">
-        <v>76000</v>
+        <v>83200</v>
       </c>
       <c r="D7" t="n">
-        <v>78800</v>
+        <v>86300</v>
       </c>
       <c r="E7" t="n">
         <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>83600</v>
+        <v>91520</v>
       </c>
       <c r="G7" t="n">
-        <v>86680</v>
+        <v>94930</v>
       </c>
       <c r="H7" t="n">
-        <v>3080</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="8">
@@ -653,22 +653,22 @@
         <v>6600</v>
       </c>
       <c r="C8" t="n">
-        <v>76000</v>
+        <v>83200</v>
       </c>
       <c r="D8" t="n">
-        <v>78800</v>
+        <v>86300</v>
       </c>
       <c r="E8" t="n">
         <v>10</v>
       </c>
       <c r="F8" t="n">
-        <v>83600</v>
+        <v>91520</v>
       </c>
       <c r="G8" t="n">
-        <v>86680</v>
+        <v>94930</v>
       </c>
       <c r="H8" t="n">
-        <v>3080</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="9">
@@ -681,22 +681,22 @@
         <v>6600</v>
       </c>
       <c r="C9" t="n">
-        <v>76000</v>
+        <v>83200</v>
       </c>
       <c r="D9" t="n">
-        <v>78800</v>
+        <v>86300</v>
       </c>
       <c r="E9" t="n">
         <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>83600</v>
+        <v>91520</v>
       </c>
       <c r="G9" t="n">
-        <v>86680</v>
+        <v>94930</v>
       </c>
       <c r="H9" t="n">
-        <v>3080</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="10">
@@ -709,22 +709,22 @@
         <v>6600</v>
       </c>
       <c r="C10" t="n">
-        <v>76000</v>
+        <v>85700</v>
       </c>
       <c r="D10" t="n">
-        <v>78800</v>
+        <v>88900</v>
       </c>
       <c r="E10" t="n">
         <v>10</v>
       </c>
       <c r="F10" t="n">
-        <v>83600</v>
+        <v>94270</v>
       </c>
       <c r="G10" t="n">
-        <v>86680</v>
+        <v>97790</v>
       </c>
       <c r="H10" t="n">
-        <v>3080</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="11">
@@ -737,22 +737,22 @@
         <v>6600</v>
       </c>
       <c r="C11" t="n">
-        <v>76000</v>
+        <v>85700</v>
       </c>
       <c r="D11" t="n">
-        <v>78800</v>
+        <v>88900</v>
       </c>
       <c r="E11" t="n">
         <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>83600</v>
+        <v>94270</v>
       </c>
       <c r="G11" t="n">
-        <v>86680</v>
+        <v>97790</v>
       </c>
       <c r="H11" t="n">
-        <v>3080</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="12">
@@ -765,22 +765,22 @@
         <v>6600</v>
       </c>
       <c r="C12" t="n">
-        <v>76000</v>
+        <v>85700</v>
       </c>
       <c r="D12" t="n">
-        <v>78800</v>
+        <v>88900</v>
       </c>
       <c r="E12" t="n">
         <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>83600</v>
+        <v>94270</v>
       </c>
       <c r="G12" t="n">
-        <v>86680</v>
+        <v>97790</v>
       </c>
       <c r="H12" t="n">
-        <v>3080</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="13">
@@ -793,22 +793,22 @@
         <v>6600</v>
       </c>
       <c r="C13" t="n">
-        <v>76000</v>
+        <v>85700</v>
       </c>
       <c r="D13" t="n">
-        <v>78800</v>
+        <v>88900</v>
       </c>
       <c r="E13" t="n">
         <v>10</v>
       </c>
       <c r="F13" t="n">
-        <v>83600</v>
+        <v>94270</v>
       </c>
       <c r="G13" t="n">
-        <v>86680</v>
+        <v>97790</v>
       </c>
       <c r="H13" t="n">
-        <v>3080</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="14">
@@ -821,22 +821,22 @@
         <v>6600</v>
       </c>
       <c r="C14" t="n">
-        <v>78300</v>
+        <v>85700</v>
       </c>
       <c r="D14" t="n">
-        <v>81200</v>
+        <v>88900</v>
       </c>
       <c r="E14" t="n">
         <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>88479</v>
+        <v>96841</v>
       </c>
       <c r="G14" t="n">
-        <v>91756</v>
+        <v>100457</v>
       </c>
       <c r="H14" t="n">
-        <v>3277</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="15">
@@ -849,22 +849,22 @@
         <v>6600</v>
       </c>
       <c r="C15" t="n">
-        <v>78300</v>
+        <v>85700</v>
       </c>
       <c r="D15" t="n">
-        <v>81200</v>
+        <v>88900</v>
       </c>
       <c r="E15" t="n">
         <v>13</v>
       </c>
       <c r="F15" t="n">
-        <v>88479</v>
+        <v>96841</v>
       </c>
       <c r="G15" t="n">
-        <v>91756</v>
+        <v>100457</v>
       </c>
       <c r="H15" t="n">
-        <v>3277</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="16">
@@ -877,22 +877,22 @@
         <v>6600</v>
       </c>
       <c r="C16" t="n">
-        <v>78300</v>
+        <v>85700</v>
       </c>
       <c r="D16" t="n">
-        <v>81200</v>
+        <v>88900</v>
       </c>
       <c r="E16" t="n">
         <v>13</v>
       </c>
       <c r="F16" t="n">
-        <v>88479</v>
+        <v>96841</v>
       </c>
       <c r="G16" t="n">
-        <v>91756</v>
+        <v>100457</v>
       </c>
       <c r="H16" t="n">
-        <v>3277</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="17">
@@ -905,22 +905,22 @@
         <v>6600</v>
       </c>
       <c r="C17" t="n">
-        <v>78300</v>
+        <v>85700</v>
       </c>
       <c r="D17" t="n">
-        <v>81200</v>
+        <v>88900</v>
       </c>
       <c r="E17" t="n">
         <v>13</v>
       </c>
       <c r="F17" t="n">
-        <v>88479</v>
+        <v>96841</v>
       </c>
       <c r="G17" t="n">
-        <v>91756</v>
+        <v>100457</v>
       </c>
       <c r="H17" t="n">
-        <v>3277</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="18">
@@ -933,22 +933,22 @@
         <v>6600</v>
       </c>
       <c r="C18" t="n">
-        <v>78300</v>
+        <v>85700</v>
       </c>
       <c r="D18" t="n">
-        <v>81200</v>
+        <v>88900</v>
       </c>
       <c r="E18" t="n">
         <v>13</v>
       </c>
       <c r="F18" t="n">
-        <v>88479</v>
+        <v>96841</v>
       </c>
       <c r="G18" t="n">
-        <v>91756</v>
+        <v>100457</v>
       </c>
       <c r="H18" t="n">
-        <v>3277</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="19">
@@ -961,22 +961,22 @@
         <v>6600</v>
       </c>
       <c r="C19" t="n">
-        <v>78300</v>
+        <v>85700</v>
       </c>
       <c r="D19" t="n">
-        <v>81200</v>
+        <v>88900</v>
       </c>
       <c r="E19" t="n">
         <v>13</v>
       </c>
       <c r="F19" t="n">
-        <v>88479</v>
+        <v>96841</v>
       </c>
       <c r="G19" t="n">
-        <v>91756</v>
+        <v>100457</v>
       </c>
       <c r="H19" t="n">
-        <v>3277</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="20">
@@ -989,22 +989,22 @@
         <v>6600</v>
       </c>
       <c r="C20" t="n">
-        <v>78300</v>
+        <v>85700</v>
       </c>
       <c r="D20" t="n">
-        <v>81200</v>
+        <v>88900</v>
       </c>
       <c r="E20" t="n">
         <v>13</v>
       </c>
       <c r="F20" t="n">
-        <v>88479</v>
+        <v>96841</v>
       </c>
       <c r="G20" t="n">
-        <v>91756</v>
+        <v>100457</v>
       </c>
       <c r="H20" t="n">
-        <v>3277</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="21">
@@ -1017,22 +1017,22 @@
         <v>6600</v>
       </c>
       <c r="C21" t="n">
-        <v>78300</v>
+        <v>85700</v>
       </c>
       <c r="D21" t="n">
-        <v>81200</v>
+        <v>88900</v>
       </c>
       <c r="E21" t="n">
         <v>13</v>
       </c>
       <c r="F21" t="n">
-        <v>88479</v>
+        <v>96841</v>
       </c>
       <c r="G21" t="n">
-        <v>91756</v>
+        <v>100457</v>
       </c>
       <c r="H21" t="n">
-        <v>3277</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="22">
@@ -1045,22 +1045,22 @@
         <v>6600</v>
       </c>
       <c r="C22" t="n">
-        <v>78300</v>
+        <v>88300</v>
       </c>
       <c r="D22" t="n">
-        <v>81200</v>
+        <v>91600</v>
       </c>
       <c r="E22" t="n">
         <v>13</v>
       </c>
       <c r="F22" t="n">
-        <v>88479</v>
+        <v>99779</v>
       </c>
       <c r="G22" t="n">
-        <v>91756</v>
+        <v>103508</v>
       </c>
       <c r="H22" t="n">
-        <v>3277</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="23">
@@ -1073,22 +1073,22 @@
         <v>6600</v>
       </c>
       <c r="C23" t="n">
-        <v>78300</v>
+        <v>88300</v>
       </c>
       <c r="D23" t="n">
-        <v>81200</v>
+        <v>91600</v>
       </c>
       <c r="E23" t="n">
         <v>13</v>
       </c>
       <c r="F23" t="n">
-        <v>88479</v>
+        <v>99779</v>
       </c>
       <c r="G23" t="n">
-        <v>91756</v>
+        <v>103508</v>
       </c>
       <c r="H23" t="n">
-        <v>3277</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="24">
@@ -1101,22 +1101,22 @@
         <v>6600</v>
       </c>
       <c r="C24" t="n">
-        <v>78300</v>
+        <v>88300</v>
       </c>
       <c r="D24" t="n">
-        <v>81200</v>
+        <v>91600</v>
       </c>
       <c r="E24" t="n">
         <v>13</v>
       </c>
       <c r="F24" t="n">
-        <v>88479</v>
+        <v>99779</v>
       </c>
       <c r="G24" t="n">
-        <v>91756</v>
+        <v>103508</v>
       </c>
       <c r="H24" t="n">
-        <v>3277</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="25">
@@ -1129,22 +1129,22 @@
         <v>6600</v>
       </c>
       <c r="C25" t="n">
-        <v>78300</v>
+        <v>88300</v>
       </c>
       <c r="D25" t="n">
-        <v>81200</v>
+        <v>91600</v>
       </c>
       <c r="E25" t="n">
         <v>13</v>
       </c>
       <c r="F25" t="n">
-        <v>88479</v>
+        <v>99779</v>
       </c>
       <c r="G25" t="n">
-        <v>91756</v>
+        <v>103508</v>
       </c>
       <c r="H25" t="n">
-        <v>3277</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="26">
@@ -1157,22 +1157,22 @@
         <v>6600</v>
       </c>
       <c r="C26" t="n">
-        <v>80700</v>
+        <v>88300</v>
       </c>
       <c r="D26" t="n">
-        <v>83700</v>
+        <v>91600</v>
       </c>
       <c r="E26" t="n">
         <v>13</v>
       </c>
       <c r="F26" t="n">
-        <v>91191</v>
+        <v>99779</v>
       </c>
       <c r="G26" t="n">
-        <v>94581</v>
+        <v>103508</v>
       </c>
       <c r="H26" t="n">
-        <v>3390</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="27">
@@ -1185,22 +1185,22 @@
         <v>6600</v>
       </c>
       <c r="C27" t="n">
-        <v>80700</v>
+        <v>88300</v>
       </c>
       <c r="D27" t="n">
-        <v>83700</v>
+        <v>91600</v>
       </c>
       <c r="E27" t="n">
         <v>13</v>
       </c>
       <c r="F27" t="n">
-        <v>91191</v>
+        <v>99779</v>
       </c>
       <c r="G27" t="n">
-        <v>94581</v>
+        <v>103508</v>
       </c>
       <c r="H27" t="n">
-        <v>3390</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="28">
@@ -1213,22 +1213,22 @@
         <v>6600</v>
       </c>
       <c r="C28" t="n">
-        <v>80700</v>
+        <v>88300</v>
       </c>
       <c r="D28" t="n">
-        <v>83700</v>
+        <v>91600</v>
       </c>
       <c r="E28" t="n">
         <v>13</v>
       </c>
       <c r="F28" t="n">
-        <v>91191</v>
+        <v>99779</v>
       </c>
       <c r="G28" t="n">
-        <v>94581</v>
+        <v>103508</v>
       </c>
       <c r="H28" t="n">
-        <v>3390</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="29">
@@ -1241,22 +1241,22 @@
         <v>6600</v>
       </c>
       <c r="C29" t="n">
-        <v>80700</v>
+        <v>88300</v>
       </c>
       <c r="D29" t="n">
-        <v>83700</v>
+        <v>91600</v>
       </c>
       <c r="E29" t="n">
         <v>13</v>
       </c>
       <c r="F29" t="n">
-        <v>91191</v>
+        <v>99779</v>
       </c>
       <c r="G29" t="n">
-        <v>94581</v>
+        <v>103508</v>
       </c>
       <c r="H29" t="n">
-        <v>3390</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="30">
@@ -1269,22 +1269,22 @@
         <v>6600</v>
       </c>
       <c r="C30" t="n">
-        <v>80700</v>
+        <v>88300</v>
       </c>
       <c r="D30" t="n">
-        <v>83700</v>
+        <v>91600</v>
       </c>
       <c r="E30" t="n">
         <v>13</v>
       </c>
       <c r="F30" t="n">
-        <v>91191</v>
+        <v>99779</v>
       </c>
       <c r="G30" t="n">
-        <v>94581</v>
+        <v>103508</v>
       </c>
       <c r="H30" t="n">
-        <v>3390</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="31">
@@ -1297,22 +1297,22 @@
         <v>6600</v>
       </c>
       <c r="C31" t="n">
-        <v>80700</v>
+        <v>88300</v>
       </c>
       <c r="D31" t="n">
-        <v>83700</v>
+        <v>91600</v>
       </c>
       <c r="E31" t="n">
         <v>13</v>
       </c>
       <c r="F31" t="n">
-        <v>91191</v>
+        <v>99779</v>
       </c>
       <c r="G31" t="n">
-        <v>94581</v>
+        <v>103508</v>
       </c>
       <c r="H31" t="n">
-        <v>3390</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="32">
@@ -1325,22 +1325,22 @@
         <v>6600</v>
       </c>
       <c r="C32" t="n">
-        <v>80700</v>
+        <v>88300</v>
       </c>
       <c r="D32" t="n">
-        <v>83700</v>
+        <v>91600</v>
       </c>
       <c r="E32" t="n">
         <v>13</v>
       </c>
       <c r="F32" t="n">
-        <v>91191</v>
+        <v>99779</v>
       </c>
       <c r="G32" t="n">
-        <v>94581</v>
+        <v>103508</v>
       </c>
       <c r="H32" t="n">
-        <v>3390</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="33">
@@ -1353,22 +1353,22 @@
         <v>6600</v>
       </c>
       <c r="C33" t="n">
-        <v>80700</v>
+        <v>88300</v>
       </c>
       <c r="D33" t="n">
-        <v>83700</v>
+        <v>91600</v>
       </c>
       <c r="E33" t="n">
         <v>13</v>
       </c>
       <c r="F33" t="n">
-        <v>91191</v>
+        <v>99779</v>
       </c>
       <c r="G33" t="n">
-        <v>94581</v>
+        <v>103508</v>
       </c>
       <c r="H33" t="n">
-        <v>3390</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="34">
@@ -1381,22 +1381,22 @@
         <v>6600</v>
       </c>
       <c r="C34" t="n">
-        <v>80700</v>
+        <v>91000</v>
       </c>
       <c r="D34" t="n">
-        <v>83700</v>
+        <v>94400</v>
       </c>
       <c r="E34" t="n">
         <v>13</v>
       </c>
       <c r="F34" t="n">
-        <v>91191</v>
+        <v>102830</v>
       </c>
       <c r="G34" t="n">
-        <v>94581</v>
+        <v>106672</v>
       </c>
       <c r="H34" t="n">
-        <v>3390</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="35">
@@ -1409,22 +1409,22 @@
         <v>6600</v>
       </c>
       <c r="C35" t="n">
-        <v>80700</v>
+        <v>91000</v>
       </c>
       <c r="D35" t="n">
-        <v>83700</v>
+        <v>94400</v>
       </c>
       <c r="E35" t="n">
         <v>13</v>
       </c>
       <c r="F35" t="n">
-        <v>91191</v>
+        <v>102830</v>
       </c>
       <c r="G35" t="n">
-        <v>94581</v>
+        <v>106672</v>
       </c>
       <c r="H35" t="n">
-        <v>3390</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="36">
@@ -1437,22 +1437,22 @@
         <v>6600</v>
       </c>
       <c r="C36" t="n">
-        <v>80700</v>
+        <v>91000</v>
       </c>
       <c r="D36" t="n">
-        <v>83700</v>
+        <v>94400</v>
       </c>
       <c r="E36" t="n">
         <v>13</v>
       </c>
       <c r="F36" t="n">
-        <v>91191</v>
+        <v>102830</v>
       </c>
       <c r="G36" t="n">
-        <v>94581</v>
+        <v>106672</v>
       </c>
       <c r="H36" t="n">
-        <v>3390</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="37">
@@ -1465,22 +1465,22 @@
         <v>6600</v>
       </c>
       <c r="C37" t="n">
-        <v>80700</v>
+        <v>91000</v>
       </c>
       <c r="D37" t="n">
-        <v>83700</v>
+        <v>94400</v>
       </c>
       <c r="E37" t="n">
         <v>13</v>
       </c>
       <c r="F37" t="n">
-        <v>91191</v>
+        <v>102830</v>
       </c>
       <c r="G37" t="n">
-        <v>94581</v>
+        <v>106672</v>
       </c>
       <c r="H37" t="n">
-        <v>3390</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="38">
@@ -1493,22 +1493,22 @@
         <v>6600</v>
       </c>
       <c r="C38" t="n">
-        <v>83200</v>
+        <v>91000</v>
       </c>
       <c r="D38" t="n">
-        <v>86300</v>
+        <v>94400</v>
       </c>
       <c r="E38" t="n">
         <v>13</v>
       </c>
       <c r="F38" t="n">
-        <v>94016</v>
+        <v>102830</v>
       </c>
       <c r="G38" t="n">
-        <v>97519</v>
+        <v>106672</v>
       </c>
       <c r="H38" t="n">
-        <v>3503</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="39">
@@ -1521,22 +1521,22 @@
         <v>6600</v>
       </c>
       <c r="C39" t="n">
-        <v>83200</v>
+        <v>91000</v>
       </c>
       <c r="D39" t="n">
-        <v>86300</v>
+        <v>94400</v>
       </c>
       <c r="E39" t="n">
         <v>13</v>
       </c>
       <c r="F39" t="n">
-        <v>94016</v>
+        <v>102830</v>
       </c>
       <c r="G39" t="n">
-        <v>97519</v>
+        <v>106672</v>
       </c>
       <c r="H39" t="n">
-        <v>3503</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="40">
@@ -1549,22 +1549,22 @@
         <v>6600</v>
       </c>
       <c r="C40" t="n">
-        <v>83200</v>
+        <v>91000</v>
       </c>
       <c r="D40" t="n">
-        <v>86300</v>
+        <v>94400</v>
       </c>
       <c r="E40" t="n">
         <v>16</v>
       </c>
       <c r="F40" t="n">
-        <v>96512</v>
+        <v>105560</v>
       </c>
       <c r="G40" t="n">
-        <v>100108</v>
+        <v>109504</v>
       </c>
       <c r="H40" t="n">
-        <v>3596</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="41">
@@ -1577,22 +1577,22 @@
         <v>6600</v>
       </c>
       <c r="C41" t="n">
-        <v>83200</v>
+        <v>91000</v>
       </c>
       <c r="D41" t="n">
-        <v>86300</v>
+        <v>94400</v>
       </c>
       <c r="E41" t="n">
         <v>16</v>
       </c>
       <c r="F41" t="n">
-        <v>96512</v>
+        <v>105560</v>
       </c>
       <c r="G41" t="n">
-        <v>100108</v>
+        <v>109504</v>
       </c>
       <c r="H41" t="n">
-        <v>3596</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="42">
@@ -1605,22 +1605,22 @@
         <v>6600</v>
       </c>
       <c r="C42" t="n">
-        <v>83200</v>
+        <v>91000</v>
       </c>
       <c r="D42" t="n">
-        <v>86300</v>
+        <v>94400</v>
       </c>
       <c r="E42" t="n">
         <v>16</v>
       </c>
       <c r="F42" t="n">
-        <v>96512</v>
+        <v>105560</v>
       </c>
       <c r="G42" t="n">
-        <v>100108</v>
+        <v>109504</v>
       </c>
       <c r="H42" t="n">
-        <v>3596</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="43">
@@ -1633,22 +1633,22 @@
         <v>6600</v>
       </c>
       <c r="C43" t="n">
-        <v>83200</v>
+        <v>91000</v>
       </c>
       <c r="D43" t="n">
-        <v>86300</v>
+        <v>94400</v>
       </c>
       <c r="E43" t="n">
         <v>16</v>
       </c>
       <c r="F43" t="n">
-        <v>96512</v>
+        <v>105560</v>
       </c>
       <c r="G43" t="n">
-        <v>100108</v>
+        <v>109504</v>
       </c>
       <c r="H43" t="n">
-        <v>3596</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="44">
@@ -1661,22 +1661,22 @@
         <v>6600</v>
       </c>
       <c r="C44" t="n">
-        <v>83200</v>
+        <v>91000</v>
       </c>
       <c r="D44" t="n">
-        <v>86300</v>
+        <v>94400</v>
       </c>
       <c r="E44" t="n">
         <v>16</v>
       </c>
       <c r="F44" t="n">
-        <v>96512</v>
+        <v>105560</v>
       </c>
       <c r="G44" t="n">
-        <v>100108</v>
+        <v>109504</v>
       </c>
       <c r="H44" t="n">
-        <v>3596</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="45">
@@ -1689,22 +1689,22 @@
         <v>6600</v>
       </c>
       <c r="C45" t="n">
-        <v>83200</v>
+        <v>91000</v>
       </c>
       <c r="D45" t="n">
-        <v>86300</v>
+        <v>94400</v>
       </c>
       <c r="E45" t="n">
         <v>16</v>
       </c>
       <c r="F45" t="n">
-        <v>96512</v>
+        <v>105560</v>
       </c>
       <c r="G45" t="n">
-        <v>100108</v>
+        <v>109504</v>
       </c>
       <c r="H45" t="n">
-        <v>3596</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="46">
@@ -1714,25 +1714,25 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C46" t="n">
-        <v>83200</v>
+        <v>99800</v>
       </c>
       <c r="D46" t="n">
-        <v>86300</v>
+        <v>105700</v>
       </c>
       <c r="E46" t="n">
         <v>16</v>
       </c>
       <c r="F46" t="n">
-        <v>96512</v>
+        <v>115768</v>
       </c>
       <c r="G46" t="n">
-        <v>100108</v>
+        <v>122612</v>
       </c>
       <c r="H46" t="n">
-        <v>3596</v>
+        <v>6844</v>
       </c>
     </row>
     <row r="47">
@@ -1742,25 +1742,25 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C47" t="n">
-        <v>83200</v>
+        <v>99800</v>
       </c>
       <c r="D47" t="n">
-        <v>86300</v>
+        <v>105700</v>
       </c>
       <c r="E47" t="n">
         <v>16</v>
       </c>
       <c r="F47" t="n">
-        <v>96512</v>
+        <v>115768</v>
       </c>
       <c r="G47" t="n">
-        <v>100108</v>
+        <v>122612</v>
       </c>
       <c r="H47" t="n">
-        <v>3596</v>
+        <v>6844</v>
       </c>
     </row>
     <row r="48">
@@ -1770,25 +1770,25 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C48" t="n">
-        <v>83200</v>
+        <v>99800</v>
       </c>
       <c r="D48" t="n">
-        <v>86300</v>
+        <v>105700</v>
       </c>
       <c r="E48" t="n">
         <v>16</v>
       </c>
       <c r="F48" t="n">
-        <v>96512</v>
+        <v>115768</v>
       </c>
       <c r="G48" t="n">
-        <v>100108</v>
+        <v>122612</v>
       </c>
       <c r="H48" t="n">
-        <v>3596</v>
+        <v>6844</v>
       </c>
     </row>
     <row r="49">
@@ -1798,25 +1798,25 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C49" t="n">
-        <v>83200</v>
+        <v>99800</v>
       </c>
       <c r="D49" t="n">
-        <v>86300</v>
+        <v>105700</v>
       </c>
       <c r="E49" t="n">
         <v>16</v>
       </c>
       <c r="F49" t="n">
-        <v>96512</v>
+        <v>115768</v>
       </c>
       <c r="G49" t="n">
-        <v>100108</v>
+        <v>122612</v>
       </c>
       <c r="H49" t="n">
-        <v>3596</v>
+        <v>6844</v>
       </c>
     </row>
     <row r="50">
@@ -1826,25 +1826,25 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C50" t="n">
-        <v>85700</v>
+        <v>99800</v>
       </c>
       <c r="D50" t="n">
-        <v>88900</v>
+        <v>105700</v>
       </c>
       <c r="E50" t="n">
         <v>20</v>
       </c>
       <c r="F50" t="n">
-        <v>102840</v>
+        <v>119760</v>
       </c>
       <c r="G50" t="n">
-        <v>106680</v>
+        <v>126840</v>
       </c>
       <c r="H50" t="n">
-        <v>3840</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="51">
@@ -1854,25 +1854,25 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C51" t="n">
-        <v>85700</v>
+        <v>99800</v>
       </c>
       <c r="D51" t="n">
-        <v>88900</v>
+        <v>105700</v>
       </c>
       <c r="E51" t="n">
         <v>20</v>
       </c>
       <c r="F51" t="n">
-        <v>102840</v>
+        <v>119760</v>
       </c>
       <c r="G51" t="n">
-        <v>106680</v>
+        <v>126840</v>
       </c>
       <c r="H51" t="n">
-        <v>3840</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="52">
@@ -1882,25 +1882,25 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C52" t="n">
-        <v>85700</v>
+        <v>99800</v>
       </c>
       <c r="D52" t="n">
-        <v>88900</v>
+        <v>105700</v>
       </c>
       <c r="E52" t="n">
         <v>20</v>
       </c>
       <c r="F52" t="n">
-        <v>102840</v>
+        <v>119760</v>
       </c>
       <c r="G52" t="n">
-        <v>106680</v>
+        <v>126840</v>
       </c>
       <c r="H52" t="n">
-        <v>3840</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="53">
@@ -1910,25 +1910,25 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C53" t="n">
-        <v>85700</v>
+        <v>99800</v>
       </c>
       <c r="D53" t="n">
-        <v>88900</v>
+        <v>105700</v>
       </c>
       <c r="E53" t="n">
         <v>24</v>
       </c>
       <c r="F53" t="n">
-        <v>106268</v>
+        <v>123752</v>
       </c>
       <c r="G53" t="n">
-        <v>110236</v>
+        <v>131068</v>
       </c>
       <c r="H53" t="n">
-        <v>3968</v>
+        <v>7316</v>
       </c>
     </row>
     <row r="54">
@@ -1938,25 +1938,25 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C54" t="n">
-        <v>85700</v>
+        <v>99800</v>
       </c>
       <c r="D54" t="n">
-        <v>88900</v>
+        <v>105700</v>
       </c>
       <c r="E54" t="n">
         <v>24</v>
       </c>
       <c r="F54" t="n">
-        <v>106268</v>
+        <v>123752</v>
       </c>
       <c r="G54" t="n">
-        <v>110236</v>
+        <v>131068</v>
       </c>
       <c r="H54" t="n">
-        <v>3968</v>
+        <v>7316</v>
       </c>
     </row>
     <row r="55">
@@ -1966,25 +1966,25 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C55" t="n">
-        <v>85700</v>
+        <v>99800</v>
       </c>
       <c r="D55" t="n">
-        <v>88900</v>
+        <v>105700</v>
       </c>
       <c r="E55" t="n">
         <v>24</v>
       </c>
       <c r="F55" t="n">
-        <v>106268</v>
+        <v>123752</v>
       </c>
       <c r="G55" t="n">
-        <v>110236</v>
+        <v>131068</v>
       </c>
       <c r="H55" t="n">
-        <v>3968</v>
+        <v>7316</v>
       </c>
     </row>
     <row r="56">
@@ -1994,25 +1994,25 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C56" t="n">
-        <v>85700</v>
+        <v>99800</v>
       </c>
       <c r="D56" t="n">
-        <v>88900</v>
+        <v>105700</v>
       </c>
       <c r="E56" t="n">
         <v>24</v>
       </c>
       <c r="F56" t="n">
-        <v>106268</v>
+        <v>123752</v>
       </c>
       <c r="G56" t="n">
-        <v>110236</v>
+        <v>131068</v>
       </c>
       <c r="H56" t="n">
-        <v>3968</v>
+        <v>7316</v>
       </c>
     </row>
     <row r="57">
@@ -2022,25 +2022,25 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C57" t="n">
-        <v>85700</v>
+        <v>99800</v>
       </c>
       <c r="D57" t="n">
-        <v>88900</v>
+        <v>105700</v>
       </c>
       <c r="E57" t="n">
         <v>24</v>
       </c>
       <c r="F57" t="n">
-        <v>106268</v>
+        <v>123752</v>
       </c>
       <c r="G57" t="n">
-        <v>110236</v>
+        <v>131068</v>
       </c>
       <c r="H57" t="n">
-        <v>3968</v>
+        <v>7316</v>
       </c>
     </row>
     <row r="58">
@@ -2050,25 +2050,25 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C58" t="n">
-        <v>85700</v>
+        <v>102800</v>
       </c>
       <c r="D58" t="n">
-        <v>88900</v>
+        <v>108900</v>
       </c>
       <c r="E58" t="n">
         <v>24</v>
       </c>
       <c r="F58" t="n">
-        <v>106268</v>
+        <v>127472</v>
       </c>
       <c r="G58" t="n">
-        <v>110236</v>
+        <v>135036</v>
       </c>
       <c r="H58" t="n">
-        <v>3968</v>
+        <v>7564</v>
       </c>
     </row>
     <row r="59">
@@ -2078,25 +2078,25 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C59" t="n">
-        <v>85700</v>
+        <v>102800</v>
       </c>
       <c r="D59" t="n">
-        <v>88900</v>
+        <v>108900</v>
       </c>
       <c r="E59" t="n">
         <v>24</v>
       </c>
       <c r="F59" t="n">
-        <v>106268</v>
+        <v>127472</v>
       </c>
       <c r="G59" t="n">
-        <v>110236</v>
+        <v>135036</v>
       </c>
       <c r="H59" t="n">
-        <v>3968</v>
+        <v>7564</v>
       </c>
     </row>
     <row r="60">
@@ -2106,25 +2106,25 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C60" t="n">
-        <v>85700</v>
+        <v>102800</v>
       </c>
       <c r="D60" t="n">
-        <v>88900</v>
+        <v>108900</v>
       </c>
       <c r="E60" t="n">
         <v>24</v>
       </c>
       <c r="F60" t="n">
-        <v>106268</v>
+        <v>127472</v>
       </c>
       <c r="G60" t="n">
-        <v>110236</v>
+        <v>135036</v>
       </c>
       <c r="H60" t="n">
-        <v>3968</v>
+        <v>7564</v>
       </c>
     </row>
     <row r="61">
@@ -2134,25 +2134,25 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C61" t="n">
-        <v>85700</v>
+        <v>102800</v>
       </c>
       <c r="D61" t="n">
-        <v>88900</v>
+        <v>108900</v>
       </c>
       <c r="E61" t="n">
         <v>24</v>
       </c>
       <c r="F61" t="n">
-        <v>106268</v>
+        <v>127472</v>
       </c>
       <c r="G61" t="n">
-        <v>110236</v>
+        <v>135036</v>
       </c>
       <c r="H61" t="n">
-        <v>3968</v>
+        <v>7564</v>
       </c>
     </row>
     <row r="62">
@@ -2162,25 +2162,25 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C62" t="n">
-        <v>88300</v>
+        <v>102800</v>
       </c>
       <c r="D62" t="n">
-        <v>91600</v>
+        <v>108900</v>
       </c>
       <c r="E62" t="n">
         <v>24</v>
       </c>
       <c r="F62" t="n">
-        <v>109492</v>
+        <v>127472</v>
       </c>
       <c r="G62" t="n">
-        <v>113584</v>
+        <v>135036</v>
       </c>
       <c r="H62" t="n">
-        <v>4092</v>
+        <v>7564</v>
       </c>
     </row>
     <row r="63">
@@ -2190,25 +2190,25 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C63" t="n">
-        <v>88300</v>
+        <v>102800</v>
       </c>
       <c r="D63" t="n">
-        <v>91600</v>
+        <v>108900</v>
       </c>
       <c r="E63" t="n">
         <v>24</v>
       </c>
       <c r="F63" t="n">
-        <v>109492</v>
+        <v>127472</v>
       </c>
       <c r="G63" t="n">
-        <v>113584</v>
+        <v>135036</v>
       </c>
       <c r="H63" t="n">
-        <v>4092</v>
+        <v>7564</v>
       </c>
     </row>
     <row r="64">
@@ -2218,25 +2218,25 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C64" t="n">
-        <v>88300</v>
+        <v>102800</v>
       </c>
       <c r="D64" t="n">
-        <v>91600</v>
+        <v>108900</v>
       </c>
       <c r="E64" t="n">
         <v>24</v>
       </c>
       <c r="F64" t="n">
-        <v>109492</v>
+        <v>127472</v>
       </c>
       <c r="G64" t="n">
-        <v>113584</v>
+        <v>135036</v>
       </c>
       <c r="H64" t="n">
-        <v>4092</v>
+        <v>7564</v>
       </c>
     </row>
     <row r="65">
@@ -2246,25 +2246,25 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C65" t="n">
-        <v>88300</v>
+        <v>102800</v>
       </c>
       <c r="D65" t="n">
-        <v>91600</v>
+        <v>108900</v>
       </c>
       <c r="E65" t="n">
         <v>28</v>
       </c>
       <c r="F65" t="n">
-        <v>113024</v>
+        <v>131584</v>
       </c>
       <c r="G65" t="n">
-        <v>117248</v>
+        <v>139392</v>
       </c>
       <c r="H65" t="n">
-        <v>4224</v>
+        <v>7808</v>
       </c>
     </row>
     <row r="66">
@@ -2274,25 +2274,25 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C66" t="n">
-        <v>88300</v>
+        <v>102800</v>
       </c>
       <c r="D66" t="n">
-        <v>91600</v>
+        <v>108900</v>
       </c>
       <c r="E66" t="n">
         <v>28</v>
       </c>
       <c r="F66" t="n">
-        <v>113024</v>
+        <v>131584</v>
       </c>
       <c r="G66" t="n">
-        <v>117248</v>
+        <v>139392</v>
       </c>
       <c r="H66" t="n">
-        <v>4224</v>
+        <v>7808</v>
       </c>
     </row>
     <row r="67">
@@ -2302,25 +2302,25 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C67" t="n">
-        <v>88300</v>
+        <v>102800</v>
       </c>
       <c r="D67" t="n">
-        <v>91600</v>
+        <v>108900</v>
       </c>
       <c r="E67" t="n">
         <v>28</v>
       </c>
       <c r="F67" t="n">
-        <v>113024</v>
+        <v>131584</v>
       </c>
       <c r="G67" t="n">
-        <v>117248</v>
+        <v>139392</v>
       </c>
       <c r="H67" t="n">
-        <v>4224</v>
+        <v>7808</v>
       </c>
     </row>
     <row r="68">
@@ -2330,25 +2330,25 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C68" t="n">
-        <v>88300</v>
+        <v>102800</v>
       </c>
       <c r="D68" t="n">
-        <v>91600</v>
+        <v>108900</v>
       </c>
       <c r="E68" t="n">
         <v>28</v>
       </c>
       <c r="F68" t="n">
-        <v>113024</v>
+        <v>131584</v>
       </c>
       <c r="G68" t="n">
-        <v>117248</v>
+        <v>139392</v>
       </c>
       <c r="H68" t="n">
-        <v>4224</v>
+        <v>7808</v>
       </c>
     </row>
     <row r="69">
@@ -2358,25 +2358,25 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C69" t="n">
-        <v>88300</v>
+        <v>102800</v>
       </c>
       <c r="D69" t="n">
-        <v>91600</v>
+        <v>108900</v>
       </c>
       <c r="E69" t="n">
         <v>28</v>
       </c>
       <c r="F69" t="n">
-        <v>113024</v>
+        <v>131584</v>
       </c>
       <c r="G69" t="n">
-        <v>117248</v>
+        <v>139392</v>
       </c>
       <c r="H69" t="n">
-        <v>4224</v>
+        <v>7808</v>
       </c>
     </row>
     <row r="70">
@@ -2386,25 +2386,25 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C70" t="n">
-        <v>88300</v>
+        <v>105900</v>
       </c>
       <c r="D70" t="n">
-        <v>91600</v>
+        <v>112200</v>
       </c>
       <c r="E70" t="n">
         <v>28</v>
       </c>
       <c r="F70" t="n">
-        <v>113024</v>
+        <v>135552</v>
       </c>
       <c r="G70" t="n">
-        <v>117248</v>
+        <v>143616</v>
       </c>
       <c r="H70" t="n">
-        <v>4224</v>
+        <v>8064</v>
       </c>
     </row>
     <row r="71">
@@ -2414,25 +2414,25 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C71" t="n">
-        <v>88300</v>
+        <v>105900</v>
       </c>
       <c r="D71" t="n">
-        <v>91600</v>
+        <v>112200</v>
       </c>
       <c r="E71" t="n">
         <v>28</v>
       </c>
       <c r="F71" t="n">
-        <v>113024</v>
+        <v>135552</v>
       </c>
       <c r="G71" t="n">
-        <v>117248</v>
+        <v>143616</v>
       </c>
       <c r="H71" t="n">
-        <v>4224</v>
+        <v>8064</v>
       </c>
     </row>
     <row r="72">
@@ -2442,25 +2442,25 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C72" t="n">
-        <v>88300</v>
+        <v>105900</v>
       </c>
       <c r="D72" t="n">
-        <v>91600</v>
+        <v>112200</v>
       </c>
       <c r="E72" t="n">
         <v>28</v>
       </c>
       <c r="F72" t="n">
-        <v>113024</v>
+        <v>135552</v>
       </c>
       <c r="G72" t="n">
-        <v>117248</v>
+        <v>143616</v>
       </c>
       <c r="H72" t="n">
-        <v>4224</v>
+        <v>8064</v>
       </c>
     </row>
     <row r="73">
@@ -2470,25 +2470,25 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C73" t="n">
-        <v>88300</v>
+        <v>105900</v>
       </c>
       <c r="D73" t="n">
-        <v>91600</v>
+        <v>112200</v>
       </c>
       <c r="E73" t="n">
         <v>28</v>
       </c>
       <c r="F73" t="n">
-        <v>113024</v>
+        <v>135552</v>
       </c>
       <c r="G73" t="n">
-        <v>117248</v>
+        <v>143616</v>
       </c>
       <c r="H73" t="n">
-        <v>4224</v>
+        <v>8064</v>
       </c>
     </row>
     <row r="74">
@@ -2498,25 +2498,25 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C74" t="n">
-        <v>91000</v>
+        <v>105900</v>
       </c>
       <c r="D74" t="n">
-        <v>94400</v>
+        <v>112200</v>
       </c>
       <c r="E74" t="n">
         <v>28</v>
       </c>
       <c r="F74" t="n">
-        <v>116480</v>
+        <v>135552</v>
       </c>
       <c r="G74" t="n">
-        <v>120832</v>
+        <v>143616</v>
       </c>
       <c r="H74" t="n">
-        <v>4352</v>
+        <v>8064</v>
       </c>
     </row>
     <row r="75">
@@ -2529,22 +2529,22 @@
         <v>7600</v>
       </c>
       <c r="C75" t="n">
-        <v>96800</v>
+        <v>105900</v>
       </c>
       <c r="D75" t="n">
-        <v>102600</v>
+        <v>112200</v>
       </c>
       <c r="E75" t="n">
         <v>28</v>
       </c>
       <c r="F75" t="n">
-        <v>123904</v>
+        <v>135552</v>
       </c>
       <c r="G75" t="n">
-        <v>131328</v>
+        <v>143616</v>
       </c>
       <c r="H75" t="n">
-        <v>7424</v>
+        <v>8064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
container related warning rectified
</commit_message>
<xml_diff>
--- a/arrear_report.xlsx
+++ b/arrear_report.xlsx
@@ -485,22 +485,22 @@
         <v>6600</v>
       </c>
       <c r="C2" t="n">
-        <v>83200</v>
+        <v>78300</v>
       </c>
       <c r="D2" t="n">
-        <v>86300</v>
+        <v>81200</v>
       </c>
       <c r="E2" t="n">
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>91520</v>
+        <v>86130</v>
       </c>
       <c r="G2" t="n">
-        <v>94930</v>
+        <v>89320</v>
       </c>
       <c r="H2" t="n">
-        <v>3410</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="3">
@@ -513,22 +513,22 @@
         <v>6600</v>
       </c>
       <c r="C3" t="n">
-        <v>83200</v>
+        <v>78300</v>
       </c>
       <c r="D3" t="n">
-        <v>86300</v>
+        <v>81200</v>
       </c>
       <c r="E3" t="n">
         <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>91520</v>
+        <v>86130</v>
       </c>
       <c r="G3" t="n">
-        <v>94930</v>
+        <v>89320</v>
       </c>
       <c r="H3" t="n">
-        <v>3410</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="4">
@@ -541,22 +541,22 @@
         <v>6600</v>
       </c>
       <c r="C4" t="n">
-        <v>83200</v>
+        <v>78300</v>
       </c>
       <c r="D4" t="n">
-        <v>86300</v>
+        <v>81200</v>
       </c>
       <c r="E4" t="n">
         <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>91520</v>
+        <v>86130</v>
       </c>
       <c r="G4" t="n">
-        <v>94930</v>
+        <v>89320</v>
       </c>
       <c r="H4" t="n">
-        <v>3410</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="5">
@@ -569,22 +569,22 @@
         <v>6600</v>
       </c>
       <c r="C5" t="n">
-        <v>83200</v>
+        <v>78300</v>
       </c>
       <c r="D5" t="n">
-        <v>86300</v>
+        <v>81200</v>
       </c>
       <c r="E5" t="n">
         <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>91520</v>
+        <v>86130</v>
       </c>
       <c r="G5" t="n">
-        <v>94930</v>
+        <v>89320</v>
       </c>
       <c r="H5" t="n">
-        <v>3410</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="6">
@@ -597,22 +597,22 @@
         <v>6600</v>
       </c>
       <c r="C6" t="n">
-        <v>83200</v>
+        <v>78300</v>
       </c>
       <c r="D6" t="n">
-        <v>86300</v>
+        <v>81200</v>
       </c>
       <c r="E6" t="n">
         <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>91520</v>
+        <v>86130</v>
       </c>
       <c r="G6" t="n">
-        <v>94930</v>
+        <v>89320</v>
       </c>
       <c r="H6" t="n">
-        <v>3410</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="7">
@@ -625,22 +625,22 @@
         <v>6600</v>
       </c>
       <c r="C7" t="n">
-        <v>83200</v>
+        <v>78300</v>
       </c>
       <c r="D7" t="n">
-        <v>86300</v>
+        <v>81200</v>
       </c>
       <c r="E7" t="n">
         <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>91520</v>
+        <v>86130</v>
       </c>
       <c r="G7" t="n">
-        <v>94930</v>
+        <v>89320</v>
       </c>
       <c r="H7" t="n">
-        <v>3410</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="8">
@@ -653,22 +653,22 @@
         <v>6600</v>
       </c>
       <c r="C8" t="n">
-        <v>83200</v>
+        <v>78300</v>
       </c>
       <c r="D8" t="n">
-        <v>86300</v>
+        <v>81200</v>
       </c>
       <c r="E8" t="n">
         <v>10</v>
       </c>
       <c r="F8" t="n">
-        <v>91520</v>
+        <v>86130</v>
       </c>
       <c r="G8" t="n">
-        <v>94930</v>
+        <v>89320</v>
       </c>
       <c r="H8" t="n">
-        <v>3410</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="9">
@@ -681,22 +681,22 @@
         <v>6600</v>
       </c>
       <c r="C9" t="n">
-        <v>83200</v>
+        <v>78300</v>
       </c>
       <c r="D9" t="n">
-        <v>86300</v>
+        <v>81200</v>
       </c>
       <c r="E9" t="n">
         <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>91520</v>
+        <v>86130</v>
       </c>
       <c r="G9" t="n">
-        <v>94930</v>
+        <v>89320</v>
       </c>
       <c r="H9" t="n">
-        <v>3410</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="10">
@@ -709,22 +709,22 @@
         <v>6600</v>
       </c>
       <c r="C10" t="n">
-        <v>85700</v>
+        <v>78300</v>
       </c>
       <c r="D10" t="n">
-        <v>88900</v>
+        <v>81200</v>
       </c>
       <c r="E10" t="n">
         <v>10</v>
       </c>
       <c r="F10" t="n">
-        <v>94270</v>
+        <v>86130</v>
       </c>
       <c r="G10" t="n">
-        <v>97790</v>
+        <v>89320</v>
       </c>
       <c r="H10" t="n">
-        <v>3520</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="11">
@@ -737,22 +737,22 @@
         <v>6600</v>
       </c>
       <c r="C11" t="n">
-        <v>85700</v>
+        <v>78300</v>
       </c>
       <c r="D11" t="n">
-        <v>88900</v>
+        <v>81200</v>
       </c>
       <c r="E11" t="n">
         <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>94270</v>
+        <v>86130</v>
       </c>
       <c r="G11" t="n">
-        <v>97790</v>
+        <v>89320</v>
       </c>
       <c r="H11" t="n">
-        <v>3520</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="12">
@@ -765,22 +765,22 @@
         <v>6600</v>
       </c>
       <c r="C12" t="n">
-        <v>85700</v>
+        <v>78300</v>
       </c>
       <c r="D12" t="n">
-        <v>88900</v>
+        <v>81200</v>
       </c>
       <c r="E12" t="n">
         <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>94270</v>
+        <v>86130</v>
       </c>
       <c r="G12" t="n">
-        <v>97790</v>
+        <v>89320</v>
       </c>
       <c r="H12" t="n">
-        <v>3520</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="13">
@@ -793,22 +793,22 @@
         <v>6600</v>
       </c>
       <c r="C13" t="n">
-        <v>85700</v>
+        <v>78300</v>
       </c>
       <c r="D13" t="n">
-        <v>88900</v>
+        <v>81200</v>
       </c>
       <c r="E13" t="n">
         <v>10</v>
       </c>
       <c r="F13" t="n">
-        <v>94270</v>
+        <v>86130</v>
       </c>
       <c r="G13" t="n">
-        <v>97790</v>
+        <v>89320</v>
       </c>
       <c r="H13" t="n">
-        <v>3520</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="14">
@@ -821,22 +821,22 @@
         <v>6600</v>
       </c>
       <c r="C14" t="n">
-        <v>85700</v>
+        <v>80700</v>
       </c>
       <c r="D14" t="n">
-        <v>88900</v>
+        <v>83700</v>
       </c>
       <c r="E14" t="n">
         <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>96841</v>
+        <v>91191</v>
       </c>
       <c r="G14" t="n">
-        <v>100457</v>
+        <v>94581</v>
       </c>
       <c r="H14" t="n">
-        <v>3616</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="15">
@@ -849,22 +849,22 @@
         <v>6600</v>
       </c>
       <c r="C15" t="n">
-        <v>85700</v>
+        <v>80700</v>
       </c>
       <c r="D15" t="n">
-        <v>88900</v>
+        <v>83700</v>
       </c>
       <c r="E15" t="n">
         <v>13</v>
       </c>
       <c r="F15" t="n">
-        <v>96841</v>
+        <v>91191</v>
       </c>
       <c r="G15" t="n">
-        <v>100457</v>
+        <v>94581</v>
       </c>
       <c r="H15" t="n">
-        <v>3616</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="16">
@@ -877,22 +877,22 @@
         <v>6600</v>
       </c>
       <c r="C16" t="n">
-        <v>85700</v>
+        <v>80700</v>
       </c>
       <c r="D16" t="n">
-        <v>88900</v>
+        <v>83700</v>
       </c>
       <c r="E16" t="n">
         <v>13</v>
       </c>
       <c r="F16" t="n">
-        <v>96841</v>
+        <v>91191</v>
       </c>
       <c r="G16" t="n">
-        <v>100457</v>
+        <v>94581</v>
       </c>
       <c r="H16" t="n">
-        <v>3616</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="17">
@@ -905,22 +905,22 @@
         <v>6600</v>
       </c>
       <c r="C17" t="n">
-        <v>85700</v>
+        <v>80700</v>
       </c>
       <c r="D17" t="n">
-        <v>88900</v>
+        <v>83700</v>
       </c>
       <c r="E17" t="n">
         <v>13</v>
       </c>
       <c r="F17" t="n">
-        <v>96841</v>
+        <v>91191</v>
       </c>
       <c r="G17" t="n">
-        <v>100457</v>
+        <v>94581</v>
       </c>
       <c r="H17" t="n">
-        <v>3616</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="18">
@@ -933,22 +933,22 @@
         <v>6600</v>
       </c>
       <c r="C18" t="n">
-        <v>85700</v>
+        <v>80700</v>
       </c>
       <c r="D18" t="n">
-        <v>88900</v>
+        <v>83700</v>
       </c>
       <c r="E18" t="n">
         <v>13</v>
       </c>
       <c r="F18" t="n">
-        <v>96841</v>
+        <v>91191</v>
       </c>
       <c r="G18" t="n">
-        <v>100457</v>
+        <v>94581</v>
       </c>
       <c r="H18" t="n">
-        <v>3616</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="19">
@@ -961,22 +961,22 @@
         <v>6600</v>
       </c>
       <c r="C19" t="n">
-        <v>85700</v>
+        <v>80700</v>
       </c>
       <c r="D19" t="n">
-        <v>88900</v>
+        <v>83700</v>
       </c>
       <c r="E19" t="n">
         <v>13</v>
       </c>
       <c r="F19" t="n">
-        <v>96841</v>
+        <v>91191</v>
       </c>
       <c r="G19" t="n">
-        <v>100457</v>
+        <v>94581</v>
       </c>
       <c r="H19" t="n">
-        <v>3616</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="20">
@@ -989,22 +989,22 @@
         <v>6600</v>
       </c>
       <c r="C20" t="n">
-        <v>85700</v>
+        <v>80700</v>
       </c>
       <c r="D20" t="n">
-        <v>88900</v>
+        <v>83700</v>
       </c>
       <c r="E20" t="n">
         <v>13</v>
       </c>
       <c r="F20" t="n">
-        <v>96841</v>
+        <v>91191</v>
       </c>
       <c r="G20" t="n">
-        <v>100457</v>
+        <v>94581</v>
       </c>
       <c r="H20" t="n">
-        <v>3616</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="21">
@@ -1017,22 +1017,22 @@
         <v>6600</v>
       </c>
       <c r="C21" t="n">
-        <v>85700</v>
+        <v>80700</v>
       </c>
       <c r="D21" t="n">
-        <v>88900</v>
+        <v>83700</v>
       </c>
       <c r="E21" t="n">
         <v>13</v>
       </c>
       <c r="F21" t="n">
-        <v>96841</v>
+        <v>91191</v>
       </c>
       <c r="G21" t="n">
-        <v>100457</v>
+        <v>94581</v>
       </c>
       <c r="H21" t="n">
-        <v>3616</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="22">
@@ -1045,22 +1045,22 @@
         <v>6600</v>
       </c>
       <c r="C22" t="n">
-        <v>88300</v>
+        <v>80700</v>
       </c>
       <c r="D22" t="n">
-        <v>91600</v>
+        <v>83700</v>
       </c>
       <c r="E22" t="n">
         <v>13</v>
       </c>
       <c r="F22" t="n">
-        <v>99779</v>
+        <v>91191</v>
       </c>
       <c r="G22" t="n">
-        <v>103508</v>
+        <v>94581</v>
       </c>
       <c r="H22" t="n">
-        <v>3729</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="23">
@@ -1073,22 +1073,22 @@
         <v>6600</v>
       </c>
       <c r="C23" t="n">
-        <v>88300</v>
+        <v>80700</v>
       </c>
       <c r="D23" t="n">
-        <v>91600</v>
+        <v>83700</v>
       </c>
       <c r="E23" t="n">
         <v>13</v>
       </c>
       <c r="F23" t="n">
-        <v>99779</v>
+        <v>91191</v>
       </c>
       <c r="G23" t="n">
-        <v>103508</v>
+        <v>94581</v>
       </c>
       <c r="H23" t="n">
-        <v>3729</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="24">
@@ -1101,22 +1101,22 @@
         <v>6600</v>
       </c>
       <c r="C24" t="n">
-        <v>88300</v>
+        <v>80700</v>
       </c>
       <c r="D24" t="n">
-        <v>91600</v>
+        <v>83700</v>
       </c>
       <c r="E24" t="n">
         <v>13</v>
       </c>
       <c r="F24" t="n">
-        <v>99779</v>
+        <v>91191</v>
       </c>
       <c r="G24" t="n">
-        <v>103508</v>
+        <v>94581</v>
       </c>
       <c r="H24" t="n">
-        <v>3729</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="25">
@@ -1129,22 +1129,22 @@
         <v>6600</v>
       </c>
       <c r="C25" t="n">
-        <v>88300</v>
+        <v>80700</v>
       </c>
       <c r="D25" t="n">
-        <v>91600</v>
+        <v>83700</v>
       </c>
       <c r="E25" t="n">
         <v>13</v>
       </c>
       <c r="F25" t="n">
-        <v>99779</v>
+        <v>91191</v>
       </c>
       <c r="G25" t="n">
-        <v>103508</v>
+        <v>94581</v>
       </c>
       <c r="H25" t="n">
-        <v>3729</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="26">
@@ -1157,22 +1157,22 @@
         <v>6600</v>
       </c>
       <c r="C26" t="n">
-        <v>88300</v>
+        <v>83200</v>
       </c>
       <c r="D26" t="n">
-        <v>91600</v>
+        <v>86300</v>
       </c>
       <c r="E26" t="n">
         <v>13</v>
       </c>
       <c r="F26" t="n">
-        <v>99779</v>
+        <v>94016</v>
       </c>
       <c r="G26" t="n">
-        <v>103508</v>
+        <v>97519</v>
       </c>
       <c r="H26" t="n">
-        <v>3729</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="27">
@@ -1185,22 +1185,22 @@
         <v>6600</v>
       </c>
       <c r="C27" t="n">
-        <v>88300</v>
+        <v>83200</v>
       </c>
       <c r="D27" t="n">
-        <v>91600</v>
+        <v>86300</v>
       </c>
       <c r="E27" t="n">
         <v>13</v>
       </c>
       <c r="F27" t="n">
-        <v>99779</v>
+        <v>94016</v>
       </c>
       <c r="G27" t="n">
-        <v>103508</v>
+        <v>97519</v>
       </c>
       <c r="H27" t="n">
-        <v>3729</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="28">
@@ -1213,22 +1213,22 @@
         <v>6600</v>
       </c>
       <c r="C28" t="n">
-        <v>88300</v>
+        <v>83200</v>
       </c>
       <c r="D28" t="n">
-        <v>91600</v>
+        <v>86300</v>
       </c>
       <c r="E28" t="n">
         <v>13</v>
       </c>
       <c r="F28" t="n">
-        <v>99779</v>
+        <v>94016</v>
       </c>
       <c r="G28" t="n">
-        <v>103508</v>
+        <v>97519</v>
       </c>
       <c r="H28" t="n">
-        <v>3729</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="29">
@@ -1241,22 +1241,22 @@
         <v>6600</v>
       </c>
       <c r="C29" t="n">
-        <v>88300</v>
+        <v>83200</v>
       </c>
       <c r="D29" t="n">
-        <v>91600</v>
+        <v>86300</v>
       </c>
       <c r="E29" t="n">
         <v>13</v>
       </c>
       <c r="F29" t="n">
-        <v>99779</v>
+        <v>94016</v>
       </c>
       <c r="G29" t="n">
-        <v>103508</v>
+        <v>97519</v>
       </c>
       <c r="H29" t="n">
-        <v>3729</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="30">
@@ -1269,22 +1269,22 @@
         <v>6600</v>
       </c>
       <c r="C30" t="n">
-        <v>88300</v>
+        <v>83200</v>
       </c>
       <c r="D30" t="n">
-        <v>91600</v>
+        <v>86300</v>
       </c>
       <c r="E30" t="n">
         <v>13</v>
       </c>
       <c r="F30" t="n">
-        <v>99779</v>
+        <v>94016</v>
       </c>
       <c r="G30" t="n">
-        <v>103508</v>
+        <v>97519</v>
       </c>
       <c r="H30" t="n">
-        <v>3729</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="31">
@@ -1297,22 +1297,22 @@
         <v>6600</v>
       </c>
       <c r="C31" t="n">
-        <v>88300</v>
+        <v>83200</v>
       </c>
       <c r="D31" t="n">
-        <v>91600</v>
+        <v>86300</v>
       </c>
       <c r="E31" t="n">
         <v>13</v>
       </c>
       <c r="F31" t="n">
-        <v>99779</v>
+        <v>94016</v>
       </c>
       <c r="G31" t="n">
-        <v>103508</v>
+        <v>97519</v>
       </c>
       <c r="H31" t="n">
-        <v>3729</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="32">
@@ -1325,22 +1325,22 @@
         <v>6600</v>
       </c>
       <c r="C32" t="n">
-        <v>88300</v>
+        <v>83200</v>
       </c>
       <c r="D32" t="n">
-        <v>91600</v>
+        <v>86300</v>
       </c>
       <c r="E32" t="n">
         <v>13</v>
       </c>
       <c r="F32" t="n">
-        <v>99779</v>
+        <v>94016</v>
       </c>
       <c r="G32" t="n">
-        <v>103508</v>
+        <v>97519</v>
       </c>
       <c r="H32" t="n">
-        <v>3729</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="33">
@@ -1353,22 +1353,22 @@
         <v>6600</v>
       </c>
       <c r="C33" t="n">
-        <v>88300</v>
+        <v>83200</v>
       </c>
       <c r="D33" t="n">
-        <v>91600</v>
+        <v>86300</v>
       </c>
       <c r="E33" t="n">
         <v>13</v>
       </c>
       <c r="F33" t="n">
-        <v>99779</v>
+        <v>94016</v>
       </c>
       <c r="G33" t="n">
-        <v>103508</v>
+        <v>97519</v>
       </c>
       <c r="H33" t="n">
-        <v>3729</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="34">
@@ -1381,22 +1381,22 @@
         <v>6600</v>
       </c>
       <c r="C34" t="n">
-        <v>91000</v>
+        <v>83200</v>
       </c>
       <c r="D34" t="n">
-        <v>94400</v>
+        <v>86300</v>
       </c>
       <c r="E34" t="n">
         <v>13</v>
       </c>
       <c r="F34" t="n">
-        <v>102830</v>
+        <v>94016</v>
       </c>
       <c r="G34" t="n">
-        <v>106672</v>
+        <v>97519</v>
       </c>
       <c r="H34" t="n">
-        <v>3842</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="35">
@@ -1409,22 +1409,22 @@
         <v>6600</v>
       </c>
       <c r="C35" t="n">
-        <v>91000</v>
+        <v>83200</v>
       </c>
       <c r="D35" t="n">
-        <v>94400</v>
+        <v>86300</v>
       </c>
       <c r="E35" t="n">
         <v>13</v>
       </c>
       <c r="F35" t="n">
-        <v>102830</v>
+        <v>94016</v>
       </c>
       <c r="G35" t="n">
-        <v>106672</v>
+        <v>97519</v>
       </c>
       <c r="H35" t="n">
-        <v>3842</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="36">
@@ -1437,22 +1437,22 @@
         <v>6600</v>
       </c>
       <c r="C36" t="n">
-        <v>91000</v>
+        <v>83200</v>
       </c>
       <c r="D36" t="n">
-        <v>94400</v>
+        <v>86300</v>
       </c>
       <c r="E36" t="n">
         <v>13</v>
       </c>
       <c r="F36" t="n">
-        <v>102830</v>
+        <v>94016</v>
       </c>
       <c r="G36" t="n">
-        <v>106672</v>
+        <v>97519</v>
       </c>
       <c r="H36" t="n">
-        <v>3842</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="37">
@@ -1465,22 +1465,22 @@
         <v>6600</v>
       </c>
       <c r="C37" t="n">
-        <v>91000</v>
+        <v>83200</v>
       </c>
       <c r="D37" t="n">
-        <v>94400</v>
+        <v>86300</v>
       </c>
       <c r="E37" t="n">
         <v>13</v>
       </c>
       <c r="F37" t="n">
-        <v>102830</v>
+        <v>94016</v>
       </c>
       <c r="G37" t="n">
-        <v>106672</v>
+        <v>97519</v>
       </c>
       <c r="H37" t="n">
-        <v>3842</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="38">
@@ -1493,22 +1493,22 @@
         <v>6600</v>
       </c>
       <c r="C38" t="n">
-        <v>91000</v>
+        <v>85700</v>
       </c>
       <c r="D38" t="n">
-        <v>94400</v>
+        <v>88900</v>
       </c>
       <c r="E38" t="n">
         <v>13</v>
       </c>
       <c r="F38" t="n">
-        <v>102830</v>
+        <v>96841</v>
       </c>
       <c r="G38" t="n">
-        <v>106672</v>
+        <v>100457</v>
       </c>
       <c r="H38" t="n">
-        <v>3842</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="39">
@@ -1521,22 +1521,22 @@
         <v>6600</v>
       </c>
       <c r="C39" t="n">
-        <v>91000</v>
+        <v>85700</v>
       </c>
       <c r="D39" t="n">
-        <v>94400</v>
+        <v>88900</v>
       </c>
       <c r="E39" t="n">
         <v>13</v>
       </c>
       <c r="F39" t="n">
-        <v>102830</v>
+        <v>96841</v>
       </c>
       <c r="G39" t="n">
-        <v>106672</v>
+        <v>100457</v>
       </c>
       <c r="H39" t="n">
-        <v>3842</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="40">
@@ -1549,22 +1549,22 @@
         <v>6600</v>
       </c>
       <c r="C40" t="n">
-        <v>91000</v>
+        <v>85700</v>
       </c>
       <c r="D40" t="n">
-        <v>94400</v>
+        <v>88900</v>
       </c>
       <c r="E40" t="n">
         <v>16</v>
       </c>
       <c r="F40" t="n">
-        <v>105560</v>
+        <v>99412</v>
       </c>
       <c r="G40" t="n">
-        <v>109504</v>
+        <v>103124</v>
       </c>
       <c r="H40" t="n">
-        <v>3944</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="41">
@@ -1577,22 +1577,22 @@
         <v>6600</v>
       </c>
       <c r="C41" t="n">
-        <v>91000</v>
+        <v>85700</v>
       </c>
       <c r="D41" t="n">
-        <v>94400</v>
+        <v>88900</v>
       </c>
       <c r="E41" t="n">
         <v>16</v>
       </c>
       <c r="F41" t="n">
-        <v>105560</v>
+        <v>99412</v>
       </c>
       <c r="G41" t="n">
-        <v>109504</v>
+        <v>103124</v>
       </c>
       <c r="H41" t="n">
-        <v>3944</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="42">
@@ -1605,22 +1605,22 @@
         <v>6600</v>
       </c>
       <c r="C42" t="n">
-        <v>91000</v>
+        <v>85700</v>
       </c>
       <c r="D42" t="n">
-        <v>94400</v>
+        <v>88900</v>
       </c>
       <c r="E42" t="n">
         <v>16</v>
       </c>
       <c r="F42" t="n">
-        <v>105560</v>
+        <v>99412</v>
       </c>
       <c r="G42" t="n">
-        <v>109504</v>
+        <v>103124</v>
       </c>
       <c r="H42" t="n">
-        <v>3944</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="43">
@@ -1633,22 +1633,22 @@
         <v>6600</v>
       </c>
       <c r="C43" t="n">
-        <v>91000</v>
+        <v>85700</v>
       </c>
       <c r="D43" t="n">
-        <v>94400</v>
+        <v>88900</v>
       </c>
       <c r="E43" t="n">
         <v>16</v>
       </c>
       <c r="F43" t="n">
-        <v>105560</v>
+        <v>99412</v>
       </c>
       <c r="G43" t="n">
-        <v>109504</v>
+        <v>103124</v>
       </c>
       <c r="H43" t="n">
-        <v>3944</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="44">
@@ -1661,22 +1661,22 @@
         <v>6600</v>
       </c>
       <c r="C44" t="n">
-        <v>91000</v>
+        <v>85700</v>
       </c>
       <c r="D44" t="n">
-        <v>94400</v>
+        <v>88900</v>
       </c>
       <c r="E44" t="n">
         <v>16</v>
       </c>
       <c r="F44" t="n">
-        <v>105560</v>
+        <v>99412</v>
       </c>
       <c r="G44" t="n">
-        <v>109504</v>
+        <v>103124</v>
       </c>
       <c r="H44" t="n">
-        <v>3944</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="45">
@@ -1689,22 +1689,22 @@
         <v>6600</v>
       </c>
       <c r="C45" t="n">
-        <v>91000</v>
+        <v>85700</v>
       </c>
       <c r="D45" t="n">
-        <v>94400</v>
+        <v>88900</v>
       </c>
       <c r="E45" t="n">
         <v>16</v>
       </c>
       <c r="F45" t="n">
-        <v>105560</v>
+        <v>99412</v>
       </c>
       <c r="G45" t="n">
-        <v>109504</v>
+        <v>103124</v>
       </c>
       <c r="H45" t="n">
-        <v>3944</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="46">
@@ -1714,25 +1714,25 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C46" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D46" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E46" t="n">
         <v>16</v>
       </c>
       <c r="F46" t="n">
-        <v>115768</v>
+        <v>99412</v>
       </c>
       <c r="G46" t="n">
-        <v>122612</v>
+        <v>103124</v>
       </c>
       <c r="H46" t="n">
-        <v>6844</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="47">
@@ -1742,25 +1742,25 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C47" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D47" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E47" t="n">
         <v>16</v>
       </c>
       <c r="F47" t="n">
-        <v>115768</v>
+        <v>99412</v>
       </c>
       <c r="G47" t="n">
-        <v>122612</v>
+        <v>103124</v>
       </c>
       <c r="H47" t="n">
-        <v>6844</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="48">
@@ -1770,25 +1770,25 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C48" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D48" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E48" t="n">
         <v>16</v>
       </c>
       <c r="F48" t="n">
-        <v>115768</v>
+        <v>99412</v>
       </c>
       <c r="G48" t="n">
-        <v>122612</v>
+        <v>103124</v>
       </c>
       <c r="H48" t="n">
-        <v>6844</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="49">
@@ -1798,25 +1798,25 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C49" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D49" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E49" t="n">
         <v>16</v>
       </c>
       <c r="F49" t="n">
-        <v>115768</v>
+        <v>99412</v>
       </c>
       <c r="G49" t="n">
-        <v>122612</v>
+        <v>103124</v>
       </c>
       <c r="H49" t="n">
-        <v>6844</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="50">
@@ -2053,22 +2053,22 @@
         <v>7600</v>
       </c>
       <c r="C58" t="n">
-        <v>102800</v>
+        <v>99800</v>
       </c>
       <c r="D58" t="n">
-        <v>108900</v>
+        <v>105700</v>
       </c>
       <c r="E58" t="n">
         <v>24</v>
       </c>
       <c r="F58" t="n">
-        <v>127472</v>
+        <v>123752</v>
       </c>
       <c r="G58" t="n">
-        <v>135036</v>
+        <v>131068</v>
       </c>
       <c r="H58" t="n">
-        <v>7564</v>
+        <v>7316</v>
       </c>
     </row>
     <row r="59">
@@ -2081,22 +2081,22 @@
         <v>7600</v>
       </c>
       <c r="C59" t="n">
-        <v>102800</v>
+        <v>99800</v>
       </c>
       <c r="D59" t="n">
-        <v>108900</v>
+        <v>105700</v>
       </c>
       <c r="E59" t="n">
         <v>24</v>
       </c>
       <c r="F59" t="n">
-        <v>127472</v>
+        <v>123752</v>
       </c>
       <c r="G59" t="n">
-        <v>135036</v>
+        <v>131068</v>
       </c>
       <c r="H59" t="n">
-        <v>7564</v>
+        <v>7316</v>
       </c>
     </row>
     <row r="60">
@@ -2109,22 +2109,22 @@
         <v>7600</v>
       </c>
       <c r="C60" t="n">
-        <v>102800</v>
+        <v>99800</v>
       </c>
       <c r="D60" t="n">
-        <v>108900</v>
+        <v>105700</v>
       </c>
       <c r="E60" t="n">
         <v>24</v>
       </c>
       <c r="F60" t="n">
-        <v>127472</v>
+        <v>123752</v>
       </c>
       <c r="G60" t="n">
-        <v>135036</v>
+        <v>131068</v>
       </c>
       <c r="H60" t="n">
-        <v>7564</v>
+        <v>7316</v>
       </c>
     </row>
     <row r="61">
@@ -2137,22 +2137,22 @@
         <v>7600</v>
       </c>
       <c r="C61" t="n">
-        <v>102800</v>
+        <v>99800</v>
       </c>
       <c r="D61" t="n">
-        <v>108900</v>
+        <v>105700</v>
       </c>
       <c r="E61" t="n">
         <v>24</v>
       </c>
       <c r="F61" t="n">
-        <v>127472</v>
+        <v>123752</v>
       </c>
       <c r="G61" t="n">
-        <v>135036</v>
+        <v>131068</v>
       </c>
       <c r="H61" t="n">
-        <v>7564</v>
+        <v>7316</v>
       </c>
     </row>
     <row r="62">
@@ -2389,22 +2389,22 @@
         <v>7600</v>
       </c>
       <c r="C70" t="n">
-        <v>105900</v>
+        <v>102800</v>
       </c>
       <c r="D70" t="n">
-        <v>112200</v>
+        <v>108900</v>
       </c>
       <c r="E70" t="n">
         <v>28</v>
       </c>
       <c r="F70" t="n">
-        <v>135552</v>
+        <v>131584</v>
       </c>
       <c r="G70" t="n">
-        <v>143616</v>
+        <v>139392</v>
       </c>
       <c r="H70" t="n">
-        <v>8064</v>
+        <v>7808</v>
       </c>
     </row>
     <row r="71">
@@ -2417,22 +2417,22 @@
         <v>7600</v>
       </c>
       <c r="C71" t="n">
-        <v>105900</v>
+        <v>102800</v>
       </c>
       <c r="D71" t="n">
-        <v>112200</v>
+        <v>108900</v>
       </c>
       <c r="E71" t="n">
         <v>28</v>
       </c>
       <c r="F71" t="n">
-        <v>135552</v>
+        <v>131584</v>
       </c>
       <c r="G71" t="n">
-        <v>143616</v>
+        <v>139392</v>
       </c>
       <c r="H71" t="n">
-        <v>8064</v>
+        <v>7808</v>
       </c>
     </row>
     <row r="72">
@@ -2445,22 +2445,22 @@
         <v>7600</v>
       </c>
       <c r="C72" t="n">
-        <v>105900</v>
+        <v>102800</v>
       </c>
       <c r="D72" t="n">
-        <v>112200</v>
+        <v>108900</v>
       </c>
       <c r="E72" t="n">
         <v>28</v>
       </c>
       <c r="F72" t="n">
-        <v>135552</v>
+        <v>131584</v>
       </c>
       <c r="G72" t="n">
-        <v>143616</v>
+        <v>139392</v>
       </c>
       <c r="H72" t="n">
-        <v>8064</v>
+        <v>7808</v>
       </c>
     </row>
     <row r="73">
@@ -2473,22 +2473,22 @@
         <v>7600</v>
       </c>
       <c r="C73" t="n">
-        <v>105900</v>
+        <v>102800</v>
       </c>
       <c r="D73" t="n">
-        <v>112200</v>
+        <v>108900</v>
       </c>
       <c r="E73" t="n">
         <v>28</v>
       </c>
       <c r="F73" t="n">
-        <v>135552</v>
+        <v>131584</v>
       </c>
       <c r="G73" t="n">
-        <v>143616</v>
+        <v>139392</v>
       </c>
       <c r="H73" t="n">
-        <v>8064</v>
+        <v>7808</v>
       </c>
     </row>
     <row r="74">

</xml_diff>

<commit_message>
Validation included for both GP and Basic Pay for both 6600 and 7600
</commit_message>
<xml_diff>
--- a/arrear_report.xlsx
+++ b/arrear_report.xlsx
@@ -485,22 +485,22 @@
         <v>6600</v>
       </c>
       <c r="C2" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D2" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E2" t="n">
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G2" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H2" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="3">
@@ -513,22 +513,22 @@
         <v>6600</v>
       </c>
       <c r="C3" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D3" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E3" t="n">
         <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G3" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H3" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="4">
@@ -541,22 +541,22 @@
         <v>6600</v>
       </c>
       <c r="C4" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D4" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E4" t="n">
         <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G4" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H4" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="5">
@@ -569,22 +569,22 @@
         <v>6600</v>
       </c>
       <c r="C5" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D5" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E5" t="n">
         <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G5" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H5" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="6">
@@ -597,22 +597,22 @@
         <v>6600</v>
       </c>
       <c r="C6" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D6" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E6" t="n">
         <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G6" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H6" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="7">
@@ -625,22 +625,22 @@
         <v>6600</v>
       </c>
       <c r="C7" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D7" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E7" t="n">
         <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G7" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H7" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="8">
@@ -653,22 +653,22 @@
         <v>6600</v>
       </c>
       <c r="C8" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D8" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E8" t="n">
         <v>10</v>
       </c>
       <c r="F8" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G8" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H8" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="9">
@@ -681,22 +681,22 @@
         <v>6600</v>
       </c>
       <c r="C9" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D9" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E9" t="n">
         <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G9" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H9" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="10">
@@ -709,22 +709,22 @@
         <v>6600</v>
       </c>
       <c r="C10" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D10" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E10" t="n">
         <v>10</v>
       </c>
       <c r="F10" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G10" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H10" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="11">
@@ -737,22 +737,22 @@
         <v>6600</v>
       </c>
       <c r="C11" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D11" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E11" t="n">
         <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G11" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H11" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="12">
@@ -765,22 +765,22 @@
         <v>6600</v>
       </c>
       <c r="C12" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D12" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E12" t="n">
         <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G12" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H12" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="13">
@@ -793,22 +793,22 @@
         <v>6600</v>
       </c>
       <c r="C13" t="n">
-        <v>78300</v>
+        <v>76000</v>
       </c>
       <c r="D13" t="n">
-        <v>81200</v>
+        <v>78800</v>
       </c>
       <c r="E13" t="n">
         <v>10</v>
       </c>
       <c r="F13" t="n">
-        <v>86130</v>
+        <v>83600</v>
       </c>
       <c r="G13" t="n">
-        <v>89320</v>
+        <v>86680</v>
       </c>
       <c r="H13" t="n">
-        <v>3190</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="14">
@@ -821,22 +821,22 @@
         <v>6600</v>
       </c>
       <c r="C14" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D14" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E14" t="n">
         <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G14" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H14" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="15">
@@ -849,22 +849,22 @@
         <v>6600</v>
       </c>
       <c r="C15" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D15" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E15" t="n">
         <v>13</v>
       </c>
       <c r="F15" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G15" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H15" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="16">
@@ -877,22 +877,22 @@
         <v>6600</v>
       </c>
       <c r="C16" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D16" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E16" t="n">
         <v>13</v>
       </c>
       <c r="F16" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G16" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H16" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="17">
@@ -905,22 +905,22 @@
         <v>6600</v>
       </c>
       <c r="C17" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D17" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E17" t="n">
         <v>13</v>
       </c>
       <c r="F17" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G17" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H17" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="18">
@@ -933,22 +933,22 @@
         <v>6600</v>
       </c>
       <c r="C18" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D18" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E18" t="n">
         <v>13</v>
       </c>
       <c r="F18" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G18" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H18" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="19">
@@ -961,22 +961,22 @@
         <v>6600</v>
       </c>
       <c r="C19" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D19" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E19" t="n">
         <v>13</v>
       </c>
       <c r="F19" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G19" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H19" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="20">
@@ -989,22 +989,22 @@
         <v>6600</v>
       </c>
       <c r="C20" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D20" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E20" t="n">
         <v>13</v>
       </c>
       <c r="F20" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G20" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H20" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="21">
@@ -1017,22 +1017,22 @@
         <v>6600</v>
       </c>
       <c r="C21" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D21" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E21" t="n">
         <v>13</v>
       </c>
       <c r="F21" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G21" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H21" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="22">
@@ -1045,22 +1045,22 @@
         <v>6600</v>
       </c>
       <c r="C22" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D22" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E22" t="n">
         <v>13</v>
       </c>
       <c r="F22" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G22" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H22" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="23">
@@ -1073,22 +1073,22 @@
         <v>6600</v>
       </c>
       <c r="C23" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D23" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E23" t="n">
         <v>13</v>
       </c>
       <c r="F23" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G23" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H23" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="24">
@@ -1101,22 +1101,22 @@
         <v>6600</v>
       </c>
       <c r="C24" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D24" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E24" t="n">
         <v>13</v>
       </c>
       <c r="F24" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G24" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H24" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="25">
@@ -1129,22 +1129,22 @@
         <v>6600</v>
       </c>
       <c r="C25" t="n">
-        <v>80700</v>
+        <v>78300</v>
       </c>
       <c r="D25" t="n">
-        <v>83700</v>
+        <v>81200</v>
       </c>
       <c r="E25" t="n">
         <v>13</v>
       </c>
       <c r="F25" t="n">
-        <v>91191</v>
+        <v>88479</v>
       </c>
       <c r="G25" t="n">
-        <v>94581</v>
+        <v>91756</v>
       </c>
       <c r="H25" t="n">
-        <v>3390</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="26">
@@ -1157,22 +1157,22 @@
         <v>6600</v>
       </c>
       <c r="C26" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D26" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E26" t="n">
         <v>13</v>
       </c>
       <c r="F26" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G26" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H26" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="27">
@@ -1185,22 +1185,22 @@
         <v>6600</v>
       </c>
       <c r="C27" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D27" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E27" t="n">
         <v>13</v>
       </c>
       <c r="F27" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G27" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H27" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="28">
@@ -1213,22 +1213,22 @@
         <v>6600</v>
       </c>
       <c r="C28" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D28" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E28" t="n">
         <v>13</v>
       </c>
       <c r="F28" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G28" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H28" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="29">
@@ -1241,22 +1241,22 @@
         <v>6600</v>
       </c>
       <c r="C29" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D29" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E29" t="n">
         <v>13</v>
       </c>
       <c r="F29" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G29" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H29" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="30">
@@ -1269,22 +1269,22 @@
         <v>6600</v>
       </c>
       <c r="C30" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D30" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E30" t="n">
         <v>13</v>
       </c>
       <c r="F30" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G30" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H30" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="31">
@@ -1297,22 +1297,22 @@
         <v>6600</v>
       </c>
       <c r="C31" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D31" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E31" t="n">
         <v>13</v>
       </c>
       <c r="F31" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G31" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H31" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="32">
@@ -1325,22 +1325,22 @@
         <v>6600</v>
       </c>
       <c r="C32" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D32" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E32" t="n">
         <v>13</v>
       </c>
       <c r="F32" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G32" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H32" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="33">
@@ -1353,22 +1353,22 @@
         <v>6600</v>
       </c>
       <c r="C33" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D33" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E33" t="n">
         <v>13</v>
       </c>
       <c r="F33" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G33" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H33" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="34">
@@ -1381,22 +1381,22 @@
         <v>6600</v>
       </c>
       <c r="C34" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D34" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E34" t="n">
         <v>13</v>
       </c>
       <c r="F34" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G34" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H34" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="35">
@@ -1409,22 +1409,22 @@
         <v>6600</v>
       </c>
       <c r="C35" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D35" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E35" t="n">
         <v>13</v>
       </c>
       <c r="F35" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G35" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H35" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="36">
@@ -1437,22 +1437,22 @@
         <v>6600</v>
       </c>
       <c r="C36" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D36" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E36" t="n">
         <v>13</v>
       </c>
       <c r="F36" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G36" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H36" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="37">
@@ -1465,22 +1465,22 @@
         <v>6600</v>
       </c>
       <c r="C37" t="n">
-        <v>83200</v>
+        <v>80700</v>
       </c>
       <c r="D37" t="n">
-        <v>86300</v>
+        <v>83700</v>
       </c>
       <c r="E37" t="n">
         <v>13</v>
       </c>
       <c r="F37" t="n">
-        <v>94016</v>
+        <v>91191</v>
       </c>
       <c r="G37" t="n">
-        <v>97519</v>
+        <v>94581</v>
       </c>
       <c r="H37" t="n">
-        <v>3503</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="38">
@@ -1493,22 +1493,22 @@
         <v>6600</v>
       </c>
       <c r="C38" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D38" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E38" t="n">
         <v>13</v>
       </c>
       <c r="F38" t="n">
-        <v>96841</v>
+        <v>94016</v>
       </c>
       <c r="G38" t="n">
-        <v>100457</v>
+        <v>97519</v>
       </c>
       <c r="H38" t="n">
-        <v>3616</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="39">
@@ -1521,22 +1521,22 @@
         <v>6600</v>
       </c>
       <c r="C39" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D39" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E39" t="n">
         <v>13</v>
       </c>
       <c r="F39" t="n">
-        <v>96841</v>
+        <v>94016</v>
       </c>
       <c r="G39" t="n">
-        <v>100457</v>
+        <v>97519</v>
       </c>
       <c r="H39" t="n">
-        <v>3616</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="40">
@@ -1549,22 +1549,22 @@
         <v>6600</v>
       </c>
       <c r="C40" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D40" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E40" t="n">
         <v>16</v>
       </c>
       <c r="F40" t="n">
-        <v>99412</v>
+        <v>96512</v>
       </c>
       <c r="G40" t="n">
-        <v>103124</v>
+        <v>100108</v>
       </c>
       <c r="H40" t="n">
-        <v>3712</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="41">
@@ -1577,22 +1577,22 @@
         <v>6600</v>
       </c>
       <c r="C41" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D41" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E41" t="n">
         <v>16</v>
       </c>
       <c r="F41" t="n">
-        <v>99412</v>
+        <v>96512</v>
       </c>
       <c r="G41" t="n">
-        <v>103124</v>
+        <v>100108</v>
       </c>
       <c r="H41" t="n">
-        <v>3712</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="42">
@@ -1605,22 +1605,22 @@
         <v>6600</v>
       </c>
       <c r="C42" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D42" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E42" t="n">
         <v>16</v>
       </c>
       <c r="F42" t="n">
-        <v>99412</v>
+        <v>96512</v>
       </c>
       <c r="G42" t="n">
-        <v>103124</v>
+        <v>100108</v>
       </c>
       <c r="H42" t="n">
-        <v>3712</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="43">
@@ -1633,22 +1633,22 @@
         <v>6600</v>
       </c>
       <c r="C43" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D43" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E43" t="n">
         <v>16</v>
       </c>
       <c r="F43" t="n">
-        <v>99412</v>
+        <v>96512</v>
       </c>
       <c r="G43" t="n">
-        <v>103124</v>
+        <v>100108</v>
       </c>
       <c r="H43" t="n">
-        <v>3712</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="44">
@@ -1661,22 +1661,22 @@
         <v>6600</v>
       </c>
       <c r="C44" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D44" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E44" t="n">
         <v>16</v>
       </c>
       <c r="F44" t="n">
-        <v>99412</v>
+        <v>96512</v>
       </c>
       <c r="G44" t="n">
-        <v>103124</v>
+        <v>100108</v>
       </c>
       <c r="H44" t="n">
-        <v>3712</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="45">
@@ -1689,22 +1689,22 @@
         <v>6600</v>
       </c>
       <c r="C45" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D45" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E45" t="n">
         <v>16</v>
       </c>
       <c r="F45" t="n">
-        <v>99412</v>
+        <v>96512</v>
       </c>
       <c r="G45" t="n">
-        <v>103124</v>
+        <v>100108</v>
       </c>
       <c r="H45" t="n">
-        <v>3712</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="46">
@@ -1717,22 +1717,22 @@
         <v>6600</v>
       </c>
       <c r="C46" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D46" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E46" t="n">
         <v>16</v>
       </c>
       <c r="F46" t="n">
-        <v>99412</v>
+        <v>96512</v>
       </c>
       <c r="G46" t="n">
-        <v>103124</v>
+        <v>100108</v>
       </c>
       <c r="H46" t="n">
-        <v>3712</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="47">
@@ -1745,22 +1745,22 @@
         <v>6600</v>
       </c>
       <c r="C47" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D47" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E47" t="n">
         <v>16</v>
       </c>
       <c r="F47" t="n">
-        <v>99412</v>
+        <v>96512</v>
       </c>
       <c r="G47" t="n">
-        <v>103124</v>
+        <v>100108</v>
       </c>
       <c r="H47" t="n">
-        <v>3712</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="48">
@@ -1773,22 +1773,22 @@
         <v>6600</v>
       </c>
       <c r="C48" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D48" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E48" t="n">
         <v>16</v>
       </c>
       <c r="F48" t="n">
-        <v>99412</v>
+        <v>96512</v>
       </c>
       <c r="G48" t="n">
-        <v>103124</v>
+        <v>100108</v>
       </c>
       <c r="H48" t="n">
-        <v>3712</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="49">
@@ -1801,22 +1801,22 @@
         <v>6600</v>
       </c>
       <c r="C49" t="n">
-        <v>85700</v>
+        <v>83200</v>
       </c>
       <c r="D49" t="n">
-        <v>88900</v>
+        <v>86300</v>
       </c>
       <c r="E49" t="n">
         <v>16</v>
       </c>
       <c r="F49" t="n">
-        <v>99412</v>
+        <v>96512</v>
       </c>
       <c r="G49" t="n">
-        <v>103124</v>
+        <v>100108</v>
       </c>
       <c r="H49" t="n">
-        <v>3712</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="50">
@@ -1826,25 +1826,25 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C50" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D50" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E50" t="n">
         <v>20</v>
       </c>
       <c r="F50" t="n">
-        <v>119760</v>
+        <v>102840</v>
       </c>
       <c r="G50" t="n">
-        <v>126840</v>
+        <v>106680</v>
       </c>
       <c r="H50" t="n">
-        <v>7080</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="51">
@@ -1854,25 +1854,25 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C51" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D51" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E51" t="n">
         <v>20</v>
       </c>
       <c r="F51" t="n">
-        <v>119760</v>
+        <v>102840</v>
       </c>
       <c r="G51" t="n">
-        <v>126840</v>
+        <v>106680</v>
       </c>
       <c r="H51" t="n">
-        <v>7080</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="52">
@@ -1882,25 +1882,25 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C52" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D52" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E52" t="n">
         <v>20</v>
       </c>
       <c r="F52" t="n">
-        <v>119760</v>
+        <v>102840</v>
       </c>
       <c r="G52" t="n">
-        <v>126840</v>
+        <v>106680</v>
       </c>
       <c r="H52" t="n">
-        <v>7080</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="53">
@@ -1910,25 +1910,25 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C53" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D53" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E53" t="n">
         <v>24</v>
       </c>
       <c r="F53" t="n">
-        <v>123752</v>
+        <v>106268</v>
       </c>
       <c r="G53" t="n">
-        <v>131068</v>
+        <v>110236</v>
       </c>
       <c r="H53" t="n">
-        <v>7316</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="54">
@@ -1938,25 +1938,25 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C54" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D54" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E54" t="n">
         <v>24</v>
       </c>
       <c r="F54" t="n">
-        <v>123752</v>
+        <v>106268</v>
       </c>
       <c r="G54" t="n">
-        <v>131068</v>
+        <v>110236</v>
       </c>
       <c r="H54" t="n">
-        <v>7316</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="55">
@@ -1966,25 +1966,25 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C55" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D55" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E55" t="n">
         <v>24</v>
       </c>
       <c r="F55" t="n">
-        <v>123752</v>
+        <v>106268</v>
       </c>
       <c r="G55" t="n">
-        <v>131068</v>
+        <v>110236</v>
       </c>
       <c r="H55" t="n">
-        <v>7316</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="56">
@@ -1994,25 +1994,25 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C56" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D56" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E56" t="n">
         <v>24</v>
       </c>
       <c r="F56" t="n">
-        <v>123752</v>
+        <v>106268</v>
       </c>
       <c r="G56" t="n">
-        <v>131068</v>
+        <v>110236</v>
       </c>
       <c r="H56" t="n">
-        <v>7316</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="57">
@@ -2022,25 +2022,25 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C57" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D57" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E57" t="n">
         <v>24</v>
       </c>
       <c r="F57" t="n">
-        <v>123752</v>
+        <v>106268</v>
       </c>
       <c r="G57" t="n">
-        <v>131068</v>
+        <v>110236</v>
       </c>
       <c r="H57" t="n">
-        <v>7316</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="58">
@@ -2050,25 +2050,25 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C58" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D58" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E58" t="n">
         <v>24</v>
       </c>
       <c r="F58" t="n">
-        <v>123752</v>
+        <v>106268</v>
       </c>
       <c r="G58" t="n">
-        <v>131068</v>
+        <v>110236</v>
       </c>
       <c r="H58" t="n">
-        <v>7316</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="59">
@@ -2078,25 +2078,25 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C59" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D59" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E59" t="n">
         <v>24</v>
       </c>
       <c r="F59" t="n">
-        <v>123752</v>
+        <v>106268</v>
       </c>
       <c r="G59" t="n">
-        <v>131068</v>
+        <v>110236</v>
       </c>
       <c r="H59" t="n">
-        <v>7316</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="60">
@@ -2106,25 +2106,25 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C60" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D60" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E60" t="n">
         <v>24</v>
       </c>
       <c r="F60" t="n">
-        <v>123752</v>
+        <v>106268</v>
       </c>
       <c r="G60" t="n">
-        <v>131068</v>
+        <v>110236</v>
       </c>
       <c r="H60" t="n">
-        <v>7316</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="61">
@@ -2134,25 +2134,25 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C61" t="n">
-        <v>99800</v>
+        <v>85700</v>
       </c>
       <c r="D61" t="n">
-        <v>105700</v>
+        <v>88900</v>
       </c>
       <c r="E61" t="n">
         <v>24</v>
       </c>
       <c r="F61" t="n">
-        <v>123752</v>
+        <v>106268</v>
       </c>
       <c r="G61" t="n">
-        <v>131068</v>
+        <v>110236</v>
       </c>
       <c r="H61" t="n">
-        <v>7316</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="62">
@@ -2162,25 +2162,25 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C62" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D62" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E62" t="n">
         <v>24</v>
       </c>
       <c r="F62" t="n">
-        <v>127472</v>
+        <v>109492</v>
       </c>
       <c r="G62" t="n">
-        <v>135036</v>
+        <v>113584</v>
       </c>
       <c r="H62" t="n">
-        <v>7564</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="63">
@@ -2190,25 +2190,25 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C63" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D63" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E63" t="n">
         <v>24</v>
       </c>
       <c r="F63" t="n">
-        <v>127472</v>
+        <v>109492</v>
       </c>
       <c r="G63" t="n">
-        <v>135036</v>
+        <v>113584</v>
       </c>
       <c r="H63" t="n">
-        <v>7564</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="64">
@@ -2218,25 +2218,25 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C64" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D64" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E64" t="n">
         <v>24</v>
       </c>
       <c r="F64" t="n">
-        <v>127472</v>
+        <v>109492</v>
       </c>
       <c r="G64" t="n">
-        <v>135036</v>
+        <v>113584</v>
       </c>
       <c r="H64" t="n">
-        <v>7564</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="65">
@@ -2246,25 +2246,25 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C65" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D65" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E65" t="n">
         <v>28</v>
       </c>
       <c r="F65" t="n">
-        <v>131584</v>
+        <v>113024</v>
       </c>
       <c r="G65" t="n">
-        <v>139392</v>
+        <v>117248</v>
       </c>
       <c r="H65" t="n">
-        <v>7808</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="66">
@@ -2274,25 +2274,25 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C66" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D66" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E66" t="n">
         <v>28</v>
       </c>
       <c r="F66" t="n">
-        <v>131584</v>
+        <v>113024</v>
       </c>
       <c r="G66" t="n">
-        <v>139392</v>
+        <v>117248</v>
       </c>
       <c r="H66" t="n">
-        <v>7808</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="67">
@@ -2302,25 +2302,25 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C67" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D67" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E67" t="n">
         <v>28</v>
       </c>
       <c r="F67" t="n">
-        <v>131584</v>
+        <v>113024</v>
       </c>
       <c r="G67" t="n">
-        <v>139392</v>
+        <v>117248</v>
       </c>
       <c r="H67" t="n">
-        <v>7808</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="68">
@@ -2330,25 +2330,25 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C68" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D68" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E68" t="n">
         <v>28</v>
       </c>
       <c r="F68" t="n">
-        <v>131584</v>
+        <v>113024</v>
       </c>
       <c r="G68" t="n">
-        <v>139392</v>
+        <v>117248</v>
       </c>
       <c r="H68" t="n">
-        <v>7808</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="69">
@@ -2358,25 +2358,25 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C69" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D69" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E69" t="n">
         <v>28</v>
       </c>
       <c r="F69" t="n">
-        <v>131584</v>
+        <v>113024</v>
       </c>
       <c r="G69" t="n">
-        <v>139392</v>
+        <v>117248</v>
       </c>
       <c r="H69" t="n">
-        <v>7808</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="70">
@@ -2386,25 +2386,25 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C70" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D70" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E70" t="n">
         <v>28</v>
       </c>
       <c r="F70" t="n">
-        <v>131584</v>
+        <v>113024</v>
       </c>
       <c r="G70" t="n">
-        <v>139392</v>
+        <v>117248</v>
       </c>
       <c r="H70" t="n">
-        <v>7808</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="71">
@@ -2414,25 +2414,25 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C71" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D71" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E71" t="n">
         <v>28</v>
       </c>
       <c r="F71" t="n">
-        <v>131584</v>
+        <v>113024</v>
       </c>
       <c r="G71" t="n">
-        <v>139392</v>
+        <v>117248</v>
       </c>
       <c r="H71" t="n">
-        <v>7808</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="72">
@@ -2442,25 +2442,25 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C72" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D72" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E72" t="n">
         <v>28</v>
       </c>
       <c r="F72" t="n">
-        <v>131584</v>
+        <v>113024</v>
       </c>
       <c r="G72" t="n">
-        <v>139392</v>
+        <v>117248</v>
       </c>
       <c r="H72" t="n">
-        <v>7808</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="73">
@@ -2470,25 +2470,25 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C73" t="n">
-        <v>102800</v>
+        <v>88300</v>
       </c>
       <c r="D73" t="n">
-        <v>108900</v>
+        <v>91600</v>
       </c>
       <c r="E73" t="n">
         <v>28</v>
       </c>
       <c r="F73" t="n">
-        <v>131584</v>
+        <v>113024</v>
       </c>
       <c r="G73" t="n">
-        <v>139392</v>
+        <v>117248</v>
       </c>
       <c r="H73" t="n">
-        <v>7808</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="74">
@@ -2498,25 +2498,25 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C74" t="n">
-        <v>105900</v>
+        <v>91000</v>
       </c>
       <c r="D74" t="n">
-        <v>112200</v>
+        <v>94400</v>
       </c>
       <c r="E74" t="n">
         <v>28</v>
       </c>
       <c r="F74" t="n">
-        <v>135552</v>
+        <v>116480</v>
       </c>
       <c r="G74" t="n">
-        <v>143616</v>
+        <v>120832</v>
       </c>
       <c r="H74" t="n">
-        <v>8064</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="75">
@@ -2529,22 +2529,22 @@
         <v>7600</v>
       </c>
       <c r="C75" t="n">
-        <v>105900</v>
+        <v>96800</v>
       </c>
       <c r="D75" t="n">
-        <v>112200</v>
+        <v>102600</v>
       </c>
       <c r="E75" t="n">
         <v>28</v>
       </c>
       <c r="F75" t="n">
-        <v>135552</v>
+        <v>123904</v>
       </c>
       <c r="G75" t="n">
-        <v>143616</v>
+        <v>131328</v>
       </c>
       <c r="H75" t="n">
-        <v>8064</v>
+        <v>7424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised Pay Matrix download Oprion included
</commit_message>
<xml_diff>
--- a/arrear_report.xlsx
+++ b/arrear_report.xlsx
@@ -2498,25 +2498,25 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>6600</v>
+        <v>7600</v>
       </c>
       <c r="C74" t="n">
-        <v>91000</v>
+        <v>96800</v>
       </c>
       <c r="D74" t="n">
-        <v>94400</v>
+        <v>102600</v>
       </c>
       <c r="E74" t="n">
         <v>28</v>
       </c>
       <c r="F74" t="n">
-        <v>116480</v>
+        <v>123904</v>
       </c>
       <c r="G74" t="n">
-        <v>120832</v>
+        <v>131328</v>
       </c>
       <c r="H74" t="n">
-        <v>4352</v>
+        <v>7424</v>
       </c>
     </row>
     <row r="75">

</xml_diff>